<commit_message>
output variables in spreadsheet
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
     <sheet name="Setup" sheetId="7" r:id="rId2"/>
     <sheet name="Variables" sheetId="2" r:id="rId3"/>
-    <sheet name="BCL Measure Data" sheetId="10" r:id="rId4"/>
-    <sheet name="Lookups" sheetId="11" r:id="rId5"/>
+    <sheet name="Outputs" sheetId="12" r:id="rId4"/>
+    <sheet name="BCL Measure Data" sheetId="10" r:id="rId5"/>
+    <sheet name="Lookups" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$W$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$W$15</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="503">
   <si>
     <t>type</t>
   </si>
@@ -1514,6 +1516,27 @@
   </si>
   <si>
     <t>Number of worker nodes to start</t>
+  </si>
+  <si>
+    <t>Variable Display Name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>objective function</t>
+  </si>
+  <si>
+    <t>objective function target</t>
+  </si>
+  <si>
+    <t>true/false</t>
+  </si>
+  <si>
+    <t>(double)</t>
   </si>
 </sst>
 </file>
@@ -4574,17 +4597,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="1" max="1" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -4604,21 +4627,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="27"/>
       <c r="C1" s="22"/>
@@ -4627,7 +4650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>453</v>
       </c>
@@ -4636,7 +4659,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>454</v>
       </c>
@@ -4647,7 +4670,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>491</v>
       </c>
@@ -4658,7 +4681,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>468</v>
       </c>
@@ -4677,7 +4700,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>469</v>
       </c>
@@ -4696,7 +4719,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -4709,7 +4732,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="13" customFormat="1">
+    <row r="9" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>33</v>
       </c>
@@ -4718,7 +4741,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -4729,7 +4752,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -4737,7 +4760,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -4745,7 +4768,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>32</v>
       </c>
@@ -4756,7 +4779,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>486</v>
       </c>
@@ -4764,7 +4787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>480</v>
       </c>
@@ -4775,7 +4798,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -4783,7 +4806,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -4791,7 +4814,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>478</v>
       </c>
@@ -4800,7 +4823,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>38</v>
       </c>
@@ -4813,7 +4836,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -4821,7 +4844,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>35</v>
       </c>
@@ -4838,7 +4861,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28">
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
@@ -4855,7 +4878,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>40</v>
       </c>
@@ -4904,25 +4927,25 @@
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1"/>
+    <col min="7" max="7" width="11.44140625" style="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="5"/>
-    <col min="10" max="15" width="11.5" style="1"/>
-    <col min="16" max="16" width="46.1640625" style="1" customWidth="1"/>
-    <col min="17" max="19" width="11.5" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="15" width="11.44140625" style="1"/>
+    <col min="16" max="16" width="46.109375" style="1" customWidth="1"/>
+    <col min="17" max="19" width="11.44140625" style="1"/>
     <col min="20" max="20" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.5" style="1"/>
+    <col min="21" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -4950,7 +4973,7 @@
       <c r="U1" s="28"/>
       <c r="V1" s="28"/>
     </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
+    <row r="2" spans="1:22" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4963,7 +4986,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:22" s="16" customFormat="1" ht="45">
+    <row r="3" spans="1:22" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -5028,7 +5051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
@@ -5039,7 +5062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -5061,7 +5084,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -5085,7 +5108,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>25</v>
@@ -5116,7 +5139,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>26</v>
@@ -5156,7 +5179,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>25</v>
@@ -5184,7 +5207,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>25</v>
@@ -5212,7 +5235,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>25</v>
@@ -5240,7 +5263,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>25</v>
@@ -5268,7 +5291,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>25</v>
@@ -5296,7 +5319,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>25</v>
@@ -5324,7 +5347,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15" t="s">
         <v>25</v>
@@ -5352,7 +5375,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:22" customFormat="1">
+    <row r="16" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>1</v>
       </c>
@@ -5366,7 +5389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:14" customFormat="1">
+    <row r="17" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -5389,7 +5412,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:14" customFormat="1">
+    <row r="18" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -5425,7 +5448,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:14" customFormat="1">
+    <row r="19" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -5445,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" customFormat="1">
+    <row r="20" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>25</v>
       </c>
@@ -5465,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" customFormat="1">
+    <row r="21" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -5485,7 +5508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -5503,7 +5526,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23" t="s">
         <v>26</v>
@@ -5541,7 +5564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -5559,7 +5582,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" t="s">
         <v>26</v>
@@ -5597,7 +5620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -5619,7 +5642,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27" t="s">
         <v>25</v>
@@ -5644,7 +5667,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -5662,7 +5685,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29" t="s">
         <v>26</v>
@@ -5700,7 +5723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" t="s">
         <v>25</v>
@@ -5722,7 +5745,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" t="s">
         <v>25</v>
@@ -5764,25 +5787,430 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="A4:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="1"/>
+    <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="15" width="11.44140625" style="1"/>
+    <col min="16" max="16" width="46.109375" style="1" customWidth="1"/>
+    <col min="17" max="19" width="11.44140625" style="1"/>
+    <col min="20" max="20" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" s="15"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="19"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:W15"/>
+  <mergeCells count="1">
+    <mergeCell ref="Q1:V1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I327"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -5801,7 +6229,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -5822,7 +6250,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>25</v>
@@ -5845,7 +6273,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>25</v>
@@ -5868,7 +6296,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>25</v>
@@ -5891,7 +6319,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>25</v>
@@ -5914,7 +6342,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>25</v>
@@ -5937,7 +6365,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>25</v>
@@ -5960,7 +6388,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>25</v>
@@ -5983,7 +6411,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>25</v>
@@ -6006,7 +6434,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6025,7 +6453,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>25</v>
@@ -6046,7 +6474,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>25</v>
@@ -6069,7 +6497,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>25</v>
@@ -6092,7 +6520,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>25</v>
@@ -6115,7 +6543,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>25</v>
@@ -6138,7 +6566,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>25</v>
@@ -6161,7 +6589,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>25</v>
@@ -6184,7 +6612,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>25</v>
@@ -6207,7 +6635,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>25</v>
@@ -6230,7 +6658,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6249,7 +6677,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -6272,7 +6700,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>25</v>
@@ -6295,7 +6723,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>25</v>
@@ -6318,7 +6746,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -6341,7 +6769,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>25</v>
@@ -6364,7 +6792,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>25</v>
@@ -6387,7 +6815,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>25</v>
@@ -6410,7 +6838,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>25</v>
@@ -6433,7 +6861,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -6456,7 +6884,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -6475,7 +6903,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>25</v>
@@ -6496,7 +6924,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>25</v>
@@ -6519,7 +6947,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>25</v>
@@ -6542,7 +6970,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>25</v>
@@ -6565,7 +6993,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -6588,7 +7016,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>25</v>
@@ -6611,7 +7039,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>25</v>
@@ -6634,7 +7062,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>25</v>
@@ -6657,7 +7085,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>25</v>
@@ -6680,7 +7108,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -6699,7 +7127,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>25</v>
@@ -6720,7 +7148,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>25</v>
@@ -6743,7 +7171,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>25</v>
@@ -6766,7 +7194,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>25</v>
@@ -6789,7 +7217,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>25</v>
@@ -6812,7 +7240,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>25</v>
@@ -6835,7 +7263,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>25</v>
@@ -6858,7 +7286,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>25</v>
@@ -6881,7 +7309,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>25</v>
@@ -6904,7 +7332,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -6923,7 +7351,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>25</v>
@@ -6944,7 +7372,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>25</v>
@@ -6967,7 +7395,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>25</v>
@@ -6990,7 +7418,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>25</v>
@@ -7013,7 +7441,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>25</v>
@@ -7036,7 +7464,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>25</v>
@@ -7059,7 +7487,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>25</v>
@@ -7082,7 +7510,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15">
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>25</v>
@@ -7105,7 +7533,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>25</v>
@@ -7128,7 +7556,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7147,7 +7575,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>25</v>
@@ -7168,7 +7596,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>25</v>
@@ -7193,7 +7621,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>25</v>
@@ -7216,7 +7644,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>25</v>
@@ -7239,7 +7667,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>25</v>
@@ -7262,7 +7690,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>25</v>
@@ -7285,7 +7713,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>25</v>
@@ -7308,7 +7736,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>25</v>
@@ -7331,7 +7759,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>25</v>
@@ -7354,7 +7782,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>25</v>
@@ -7377,7 +7805,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -7396,7 +7824,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>25</v>
@@ -7417,7 +7845,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>25</v>
@@ -7440,7 +7868,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>25</v>
@@ -7465,7 +7893,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>25</v>
@@ -7488,7 +7916,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>25</v>
@@ -7511,7 +7939,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>25</v>
@@ -7534,7 +7962,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>25</v>
@@ -7557,7 +7985,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>25</v>
@@ -7580,7 +8008,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>25</v>
@@ -7603,7 +8031,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>25</v>
@@ -7626,7 +8054,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>25</v>
@@ -7649,7 +8077,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>25</v>
@@ -7672,7 +8100,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15">
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>25</v>
@@ -7695,7 +8123,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -7714,7 +8142,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>25</v>
@@ -7737,7 +8165,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>25</v>
@@ -7760,7 +8188,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>25</v>
@@ -7783,7 +8211,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>25</v>
@@ -7806,7 +8234,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15">
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>25</v>
@@ -7829,7 +8257,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15">
+    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>25</v>
@@ -7852,7 +8280,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>25</v>
@@ -7875,7 +8303,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15">
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>25</v>
@@ -7898,7 +8326,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15">
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>25</v>
@@ -7921,7 +8349,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15">
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>25</v>
@@ -7944,7 +8372,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -7963,7 +8391,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15">
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>25</v>
@@ -7988,7 +8416,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15">
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8007,7 +8435,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15">
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>25</v>
@@ -8028,7 +8456,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="15">
+    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>25</v>
@@ -8053,7 +8481,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15">
+    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8072,7 +8500,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15">
+    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>25</v>
@@ -8095,7 +8523,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15">
+    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>25</v>
@@ -8120,7 +8548,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15">
+    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>25</v>
@@ -8143,7 +8571,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>25</v>
@@ -8164,7 +8592,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15">
+    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8183,7 +8611,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15">
+    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>25</v>
@@ -8208,7 +8636,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15">
+    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>25</v>
@@ -8231,7 +8659,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15">
+    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>25</v>
@@ -8254,7 +8682,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>25</v>
@@ -8277,7 +8705,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15">
+    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>25</v>
@@ -8300,7 +8728,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>25</v>
@@ -8323,7 +8751,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>25</v>
@@ -8346,7 +8774,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -8365,7 +8793,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>25</v>
@@ -8388,7 +8816,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>25</v>
@@ -8411,7 +8839,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>25</v>
@@ -8434,7 +8862,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -8453,7 +8881,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>25</v>
@@ -8476,7 +8904,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>25</v>
@@ -8499,7 +8927,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15">
+    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>25</v>
@@ -8522,7 +8950,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15">
+    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>25</v>
@@ -8545,7 +8973,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15">
+    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>25</v>
@@ -8568,7 +8996,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15">
+    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>25</v>
@@ -8591,7 +9019,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15">
+    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -8610,7 +9038,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>25</v>
@@ -8635,7 +9063,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15">
+    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>25</v>
@@ -8658,7 +9086,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15">
+    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>25</v>
@@ -8681,7 +9109,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>25</v>
@@ -8704,7 +9132,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>25</v>
@@ -8727,7 +9155,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15">
+    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>25</v>
@@ -8750,7 +9178,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15">
+    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>25</v>
@@ -8773,7 +9201,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15">
+    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>25</v>
@@ -8796,7 +9224,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15">
+    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>25</v>
@@ -8819,7 +9247,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15">
+    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -8838,7 +9266,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15">
+    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>25</v>
@@ -8863,7 +9291,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15">
+    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>25</v>
@@ -8884,7 +9312,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15">
+    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>25</v>
@@ -8907,7 +9335,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15">
+    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>25</v>
@@ -8930,7 +9358,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15">
+    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>25</v>
@@ -8953,7 +9381,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15">
+    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>25</v>
@@ -8976,7 +9404,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15">
+    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>25</v>
@@ -8999,7 +9427,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15">
+    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>25</v>
@@ -9022,7 +9450,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15">
+    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>25</v>
@@ -9045,7 +9473,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15">
+    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>25</v>
@@ -9068,7 +9496,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15">
+    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>25</v>
@@ -9091,7 +9519,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15">
+    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>25</v>
@@ -9114,7 +9542,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15">
+    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>25</v>
@@ -9137,7 +9565,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15">
+    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>25</v>
@@ -9160,7 +9588,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15">
+    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9179,7 +9607,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15">
+    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>25</v>
@@ -9202,7 +9630,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15">
+    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9221,7 +9649,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15">
+    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>25</v>
@@ -9244,7 +9672,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15">
+    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>25</v>
@@ -9267,7 +9695,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9286,7 +9714,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15">
+    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>25</v>
@@ -9311,7 +9739,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15">
+    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>25</v>
@@ -9334,7 +9762,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15">
+    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>25</v>
@@ -9357,7 +9785,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15">
+    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>25</v>
@@ -9380,7 +9808,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15">
+    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>25</v>
@@ -9403,7 +9831,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15">
+    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>25</v>
@@ -9426,7 +9854,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15">
+    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>25</v>
@@ -9449,7 +9877,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15">
+    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>25</v>
@@ -9472,7 +9900,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15">
+    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>25</v>
@@ -9495,7 +9923,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15">
+    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>25</v>
@@ -9518,7 +9946,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15">
+    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -9537,7 +9965,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15">
+    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>25</v>
@@ -9562,7 +9990,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15">
+    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>25</v>
@@ -9585,7 +10013,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15">
+    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>25</v>
@@ -9608,7 +10036,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15">
+    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>25</v>
@@ -9631,7 +10059,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15">
+    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>25</v>
@@ -9654,7 +10082,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15">
+    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>25</v>
@@ -9677,7 +10105,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15">
+    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>25</v>
@@ -9700,7 +10128,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15">
+    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>25</v>
@@ -9723,7 +10151,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15">
+    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>25</v>
@@ -9746,7 +10174,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15">
+    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>25</v>
@@ -9769,7 +10197,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15">
+    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -9788,7 +10216,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15">
+    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>25</v>
@@ -9811,7 +10239,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15">
+    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>25</v>
@@ -9834,7 +10262,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15">
+    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>25</v>
@@ -9857,7 +10285,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15">
+    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>25</v>
@@ -9880,7 +10308,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15">
+    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -9899,7 +10327,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15">
+    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>25</v>
@@ -9922,7 +10350,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15">
+    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>25</v>
@@ -9945,7 +10373,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15">
+    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>25</v>
@@ -9968,7 +10396,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15">
+    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>25</v>
@@ -9991,7 +10419,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15">
+    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10010,7 +10438,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15">
+    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>25</v>
@@ -10031,7 +10459,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15">
+    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>25</v>
@@ -10054,7 +10482,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15">
+    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10073,7 +10501,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15">
+    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>25</v>
@@ -10096,7 +10524,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15">
+    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>25</v>
@@ -10121,7 +10549,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15">
+    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>25</v>
@@ -10142,7 +10570,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15">
+    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>25</v>
@@ -10167,7 +10595,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15">
+    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>25</v>
@@ -10192,7 +10620,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15">
+    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10211,7 +10639,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15">
+    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>25</v>
@@ -10236,7 +10664,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15">
+    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>25</v>
@@ -10259,7 +10687,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15">
+    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>25</v>
@@ -10282,7 +10710,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15">
+    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>25</v>
@@ -10305,7 +10733,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15">
+    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>25</v>
@@ -10328,7 +10756,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15">
+    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>25</v>
@@ -10351,7 +10779,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15">
+    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>25</v>
@@ -10374,7 +10802,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15">
+    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>25</v>
@@ -10397,7 +10825,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15">
+    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>25</v>
@@ -10420,7 +10848,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15">
+    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -10439,7 +10867,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15">
+    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>25</v>
@@ -10464,7 +10892,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15">
+    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>25</v>
@@ -10487,7 +10915,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15">
+    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>25</v>
@@ -10510,7 +10938,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15">
+    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>25</v>
@@ -10533,7 +10961,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15">
+    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>25</v>
@@ -10556,7 +10984,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15">
+    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>25</v>
@@ -10579,7 +11007,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15">
+    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>25</v>
@@ -10602,7 +11030,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15">
+    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>25</v>
@@ -10625,7 +11053,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15">
+    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>25</v>
@@ -10648,7 +11076,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15">
+    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -10667,7 +11095,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15">
+    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>25</v>
@@ -10688,7 +11116,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15">
+    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>25</v>
@@ -10711,7 +11139,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15">
+    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>25</v>
@@ -10734,7 +11162,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15">
+    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>25</v>
@@ -10757,7 +11185,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15">
+    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>25</v>
@@ -10780,7 +11208,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15">
+    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>25</v>
@@ -10803,7 +11231,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15">
+    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>25</v>
@@ -10826,7 +11254,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15">
+    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>25</v>
@@ -10849,7 +11277,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15">
+    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>25</v>
@@ -10872,7 +11300,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15">
+    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>25</v>
@@ -10895,7 +11323,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15">
+    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>25</v>
@@ -10918,7 +11346,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15">
+    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>25</v>
@@ -10941,7 +11369,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15">
+    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>25</v>
@@ -10964,7 +11392,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15">
+    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>25</v>
@@ -10987,7 +11415,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15">
+    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>25</v>
@@ -11010,7 +11438,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15">
+    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>25</v>
@@ -11033,7 +11461,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15">
+    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11052,7 +11480,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15">
+    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>25</v>
@@ -11073,7 +11501,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15">
+    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>25</v>
@@ -11096,7 +11524,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15">
+    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>25</v>
@@ -11119,7 +11547,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15">
+    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>25</v>
@@ -11142,7 +11570,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15">
+    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>25</v>
@@ -11165,7 +11593,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15">
+    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>25</v>
@@ -11188,7 +11616,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15">
+    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>25</v>
@@ -11211,7 +11639,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15">
+    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>25</v>
@@ -11234,7 +11662,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15">
+    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>25</v>
@@ -11257,7 +11685,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15">
+    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>25</v>
@@ -11280,7 +11708,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15">
+    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>25</v>
@@ -11303,7 +11731,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15">
+    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>25</v>
@@ -11326,7 +11754,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15">
+    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>25</v>
@@ -11349,7 +11777,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15">
+    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>25</v>
@@ -11372,7 +11800,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15">
+    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>25</v>
@@ -11395,7 +11823,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15">
+    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>25</v>
@@ -11418,7 +11846,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15">
+    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -11437,7 +11865,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15">
+    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>25</v>
@@ -11462,7 +11890,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15">
+    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>25</v>
@@ -11485,7 +11913,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15">
+    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>25</v>
@@ -11508,7 +11936,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15">
+    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>25</v>
@@ -11531,7 +11959,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15">
+    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>25</v>
@@ -11554,7 +11982,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15">
+    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -11573,7 +12001,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15">
+    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>25</v>
@@ -11598,7 +12026,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15">
+    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>25</v>
@@ -11621,7 +12049,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15">
+    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -11640,7 +12068,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15">
+    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -11659,7 +12087,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15">
+    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -11678,7 +12106,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15">
+    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>25</v>
@@ -11699,7 +12127,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15">
+    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>25</v>
@@ -11722,7 +12150,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15">
+    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>25</v>
@@ -11745,7 +12173,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15">
+    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>25</v>
@@ -11768,7 +12196,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15">
+    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>25</v>
@@ -11791,7 +12219,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15">
+    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>25</v>
@@ -11814,7 +12242,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15">
+    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>25</v>
@@ -11837,7 +12265,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15">
+    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>25</v>
@@ -11860,7 +12288,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15">
+    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>25</v>
@@ -11883,7 +12311,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15">
+    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>25</v>
@@ -11906,7 +12334,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15">
+    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>25</v>
@@ -11929,7 +12357,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15">
+    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -11948,7 +12376,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15">
+    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>25</v>
@@ -11971,7 +12399,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15">
+    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -11990,7 +12418,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15">
+    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>25</v>
@@ -12015,7 +12443,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15">
+    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>25</v>
@@ -12038,7 +12466,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15">
+    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>25</v>
@@ -12061,7 +12489,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15">
+    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>25</v>
@@ -12084,7 +12512,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15">
+    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>25</v>
@@ -12107,7 +12535,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15">
+    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>25</v>
@@ -12130,7 +12558,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15">
+    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>25</v>
@@ -12153,7 +12581,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15">
+    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>25</v>
@@ -12176,7 +12604,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15">
+    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>25</v>
@@ -12199,7 +12627,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15">
+    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>25</v>
@@ -12222,7 +12650,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15">
+    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>25</v>
@@ -12245,7 +12673,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15">
+    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12264,7 +12692,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15">
+    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>25</v>
@@ -12287,7 +12715,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15">
+    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12306,7 +12734,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15">
+    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>25</v>
@@ -12327,7 +12755,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15">
+    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -12346,7 +12774,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15">
+    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>25</v>
@@ -12367,7 +12795,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15">
+    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -12386,7 +12814,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15">
+    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>25</v>
@@ -12407,7 +12835,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15">
+    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -12426,7 +12854,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15">
+    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>25</v>
@@ -12449,7 +12877,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15">
+    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -12468,7 +12896,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15">
+    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>25</v>
@@ -12493,7 +12921,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15">
+    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>25</v>
@@ -12516,7 +12944,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15">
+    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>25</v>
@@ -12539,7 +12967,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15">
+    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>25</v>
@@ -12562,7 +12990,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15">
+    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>25</v>
@@ -12585,7 +13013,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15">
+    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>25</v>
@@ -12608,7 +13036,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15">
+    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>25</v>
@@ -12631,7 +13059,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15">
+    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>25</v>
@@ -12654,7 +13082,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15">
+    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>25</v>
@@ -12677,7 +13105,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15">
+    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -12696,7 +13124,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15">
+    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>25</v>
@@ -12719,7 +13147,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15">
+    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>25</v>
@@ -12742,7 +13170,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15">
+    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>25</v>
@@ -12765,7 +13193,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15">
+    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>25</v>
@@ -12788,7 +13216,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15">
+    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -12807,7 +13235,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15">
+    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>25</v>
@@ -12830,7 +13258,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15">
+    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>25</v>
@@ -12853,7 +13281,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15">
+    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>25</v>
@@ -12878,7 +13306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15">
+    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -12897,7 +13325,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15">
+    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>25</v>
@@ -12922,7 +13350,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15">
+    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>25</v>
@@ -12945,7 +13373,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15">
+    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -12964,7 +13392,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15">
+    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>25</v>
@@ -12985,7 +13413,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15">
+    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>25</v>
@@ -13006,7 +13434,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15">
+    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>25</v>
@@ -13029,7 +13457,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15">
+    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13048,7 +13476,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15">
+    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13067,7 +13495,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15">
+    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>25</v>
@@ -13092,7 +13520,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15">
+    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>25</v>
@@ -13127,7 +13555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -13135,13 +13563,13 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>467</v>
       </c>
@@ -13155,7 +13583,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -13169,7 +13597,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -13183,7 +13611,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>465</v>
       </c>
@@ -13194,7 +13622,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>459</v>
       </c>

</xml_diff>

<commit_message>
updated template and rakefile
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="509">
   <si>
     <t>type</t>
   </si>
@@ -1537,6 +1537,24 @@
   </si>
   <si>
     <t>(double)</t>
+  </si>
+  <si>
+    <t>Allow Multiple Jobs</t>
+  </si>
+  <si>
+    <t>Use Server As Worker</t>
+  </si>
+  <si>
+    <t>Simulate Data Point Filename</t>
+  </si>
+  <si>
+    <t>simulate_data_point.rb</t>
+  </si>
+  <si>
+    <t>Run Data Point Filename</t>
+  </si>
+  <si>
+    <t>run_openstudio_workflow.rb</t>
   </si>
 </sst>
 </file>
@@ -2938,7 +2956,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3003,6 +3021,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1287">
@@ -4625,16 +4646,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
@@ -4768,128 +4789,160 @@
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14" t="s">
-        <v>490</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B13" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B14" s="29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>486</v>
+        <v>505</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>480</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="14" t="s">
         <v>490</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B20" s="25">
-        <v>20</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
+        <v>486</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B24" s="25">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B27" s="25" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B29" s="26" t="s">
         <v>488</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B30" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D30" s="24" t="s">
         <v>484</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B32" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4907,7 +4960,7 @@
           <x14:formula1>
             <xm:f>Lookups!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B18</xm:sqref>
+          <xm:sqref>B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5789,7 +5842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F7" sqref="A4:F7"/>
     </sheetView>

</xml_diff>

<commit_message>
cleaning up objective functions
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16404" windowHeight="8664" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="516">
   <si>
     <t>type</t>
   </si>
@@ -1558,6 +1558,24 @@
   </si>
   <si>
     <t>Outputs</t>
+  </si>
+  <si>
+    <t>Heating Natural Gas</t>
+  </si>
+  <si>
+    <t>heating_natural_gas</t>
+  </si>
+  <si>
+    <t>MJ/m2</t>
+  </si>
+  <si>
+    <t>Cooling Electricity</t>
+  </si>
+  <si>
+    <t>cooling_electricity</t>
+  </si>
+  <si>
+    <t>MJ/m3</t>
   </si>
 </sst>
 </file>
@@ -4652,7 +4670,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5847,7 +5865,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5936,20 +5954,51 @@
       <c r="Q3" s="11"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
+      <c r="A4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>462.1635</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B5" t="s">
+        <v>514</v>
+      </c>
+      <c r="C5" t="s">
+        <v>515</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>84.162019999999998</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>

</xml_diff>

<commit_message>
call batch_run if doing LHS
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -4767,7 +4767,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4948,7 +4948,7 @@
         <v>501</v>
       </c>
       <c r="B16" s="28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>516</v>

</xml_diff>

<commit_message>
add scaling factor to template
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$I$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Y$15</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="528">
   <si>
     <t>type</t>
   </si>
@@ -1609,6 +1609,9 @@
   </si>
   <si>
     <t>1.2.0</t>
+  </si>
+  <si>
+    <t>scaling factor</t>
   </si>
 </sst>
 </file>
@@ -4736,17 +4739,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="1" max="1" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4766,21 +4769,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="27"/>
       <c r="C1" s="22"/>
@@ -4789,7 +4792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>452</v>
       </c>
@@ -4798,7 +4801,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>453</v>
       </c>
@@ -4809,7 +4812,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>488</v>
       </c>
@@ -4820,7 +4823,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>512</v>
       </c>
@@ -4831,7 +4834,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="56">
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>514</v>
       </c>
@@ -4842,7 +4845,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>466</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>467</v>
       </c>
@@ -4880,7 +4883,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>491</v>
       </c>
@@ -4893,7 +4896,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="13" customFormat="1">
+    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
@@ -4902,7 +4905,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -4913,7 +4916,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -4924,7 +4927,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -4932,7 +4935,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>500</v>
       </c>
@@ -4943,7 +4946,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>501</v>
       </c>
@@ -4954,7 +4957,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>502</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>504</v>
       </c>
@@ -4976,10 +4979,10 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" s="25"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
@@ -4990,7 +4993,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>483</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>478</v>
       </c>
@@ -5009,7 +5012,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -5017,7 +5020,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -5025,7 +5028,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>476</v>
       </c>
@@ -5034,7 +5037,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>38</v>
       </c>
@@ -5047,7 +5050,7 @@
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -5055,7 +5058,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
@@ -5072,7 +5075,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28">
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -5089,7 +5092,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>40</v>
       </c>
@@ -5138,25 +5141,25 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1"/>
+    <col min="7" max="7" width="11.44140625" style="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="5"/>
-    <col min="10" max="17" width="11.5" style="1"/>
-    <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
-    <col min="19" max="21" width="11.5" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="46.109375" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11.44140625" style="1"/>
     <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.5" style="1"/>
+    <col min="23" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -5190,7 +5193,7 @@
       <c r="W1" s="33"/>
       <c r="X1" s="33"/>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -5203,7 +5206,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" ht="45">
+    <row r="3" spans="1:24" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -5274,7 +5277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
@@ -5285,7 +5288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -5309,7 +5312,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -5335,7 +5338,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>25</v>
@@ -5368,7 +5371,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>26</v>
@@ -5410,7 +5413,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>25</v>
@@ -5440,7 +5443,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>25</v>
@@ -5470,7 +5473,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>25</v>
@@ -5500,7 +5503,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>25</v>
@@ -5530,7 +5533,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>25</v>
@@ -5560,7 +5563,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>25</v>
@@ -5590,7 +5593,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15" t="s">
         <v>25</v>
@@ -5620,7 +5623,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:24" customFormat="1">
+    <row r="16" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>1</v>
       </c>
@@ -5634,7 +5637,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:16" customFormat="1">
+    <row r="17" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -5657,7 +5660,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:16" customFormat="1">
+    <row r="18" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -5695,7 +5698,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:16" customFormat="1">
+    <row r="19" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -5715,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" customFormat="1">
+    <row r="20" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>25</v>
       </c>
@@ -5735,7 +5738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" customFormat="1">
+    <row r="21" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -5755,7 +5758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -5773,7 +5776,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23" t="s">
         <v>26</v>
@@ -5813,7 +5816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -5831,7 +5834,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" t="s">
         <v>26</v>
@@ -5871,7 +5874,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26" t="s">
         <v>25</v>
@@ -5893,7 +5896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27" t="s">
         <v>25</v>
@@ -5918,7 +5921,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -5936,7 +5939,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29" t="s">
         <v>26</v>
@@ -5976,7 +5979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" t="s">
         <v>25</v>
@@ -5998,7 +6001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" t="s">
         <v>25</v>
@@ -6042,26 +6045,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1"/>
+    <col min="7" max="7" width="11.44140625" style="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="5"/>
-    <col min="10" max="16384" width="11.5" style="1"/>
+    <col min="9" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -6074,7 +6077,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="15">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>493</v>
       </c>
@@ -6090,10 +6093,13 @@
       <c r="E2" s="9" t="s">
         <v>497</v>
       </c>
+      <c r="F2" s="9" t="s">
+        <v>527</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" s="16" customFormat="1" ht="15">
+    <row r="3" spans="1:9" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -6107,7 +6113,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>507</v>
       </c>
@@ -6123,11 +6129,14 @@
       <c r="E4">
         <v>462.1635</v>
       </c>
-      <c r="F4"/>
+      <c r="F4">
+        <f>2*E4</f>
+        <v>924.327</v>
+      </c>
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>510</v>
       </c>
@@ -6143,12 +6152,15 @@
       <c r="E5">
         <v>84.162019999999998</v>
       </c>
-      <c r="F5"/>
+      <c r="F5">
+        <f>2*E5</f>
+        <v>168.32404</v>
+      </c>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -6158,7 +6170,7 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -6169,7 +6181,7 @@
       <c r="H7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6179,7 +6191,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="15"/>
@@ -6189,7 +6201,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -6199,7 +6211,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -6209,7 +6221,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -6219,7 +6231,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -6229,7 +6241,7 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -6239,7 +6251,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -6249,15 +6261,15 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:9" customFormat="1"/>
-    <row r="17" spans="1:9" customFormat="1"/>
-    <row r="18" spans="1:9" customFormat="1">
+    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="1:9" customFormat="1"/>
-    <row r="20" spans="1:9" customFormat="1"/>
-    <row r="21" spans="1:9" customFormat="1"/>
-    <row r="22" spans="1:9">
+    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -6267,7 +6279,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -6277,7 +6289,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -6287,7 +6299,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -6297,7 +6309,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -6307,7 +6319,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -6318,7 +6330,7 @@
       <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -6328,7 +6340,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -6338,7 +6350,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -6348,7 +6360,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -6378,19 +6390,19 @@
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -6409,7 +6421,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -6430,7 +6442,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>25</v>
@@ -6453,7 +6465,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>25</v>
@@ -6476,7 +6488,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>25</v>
@@ -6499,7 +6511,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>25</v>
@@ -6522,7 +6534,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>25</v>
@@ -6545,7 +6557,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>25</v>
@@ -6568,7 +6580,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>25</v>
@@ -6591,7 +6603,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>25</v>
@@ -6614,7 +6626,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6633,7 +6645,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>25</v>
@@ -6654,7 +6666,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>25</v>
@@ -6677,7 +6689,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>25</v>
@@ -6700,7 +6712,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>25</v>
@@ -6723,7 +6735,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>25</v>
@@ -6746,7 +6758,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>25</v>
@@ -6769,7 +6781,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>25</v>
@@ -6792,7 +6804,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>25</v>
@@ -6815,7 +6827,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>25</v>
@@ -6838,7 +6850,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6857,7 +6869,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -6880,7 +6892,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>25</v>
@@ -6903,7 +6915,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>25</v>
@@ -6926,7 +6938,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -6949,7 +6961,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>25</v>
@@ -6972,7 +6984,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>25</v>
@@ -6995,7 +7007,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>25</v>
@@ -7018,7 +7030,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>25</v>
@@ -7041,7 +7053,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -7064,7 +7076,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -7083,7 +7095,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>25</v>
@@ -7104,7 +7116,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>25</v>
@@ -7127,7 +7139,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>25</v>
@@ -7150,7 +7162,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>25</v>
@@ -7173,7 +7185,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -7196,7 +7208,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>25</v>
@@ -7219,7 +7231,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>25</v>
@@ -7242,7 +7254,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>25</v>
@@ -7265,7 +7277,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>25</v>
@@ -7288,7 +7300,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -7307,7 +7319,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>25</v>
@@ -7328,7 +7340,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>25</v>
@@ -7351,7 +7363,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>25</v>
@@ -7374,7 +7386,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>25</v>
@@ -7397,7 +7409,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>25</v>
@@ -7420,7 +7432,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>25</v>
@@ -7443,7 +7455,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>25</v>
@@ -7466,7 +7478,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>25</v>
@@ -7489,7 +7501,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>25</v>
@@ -7512,7 +7524,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -7531,7 +7543,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>25</v>
@@ -7552,7 +7564,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>25</v>
@@ -7575,7 +7587,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>25</v>
@@ -7598,7 +7610,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>25</v>
@@ -7621,7 +7633,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>25</v>
@@ -7644,7 +7656,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>25</v>
@@ -7667,7 +7679,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>25</v>
@@ -7690,7 +7702,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15">
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>25</v>
@@ -7713,7 +7725,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>25</v>
@@ -7736,7 +7748,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7755,7 +7767,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>25</v>
@@ -7776,7 +7788,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>25</v>
@@ -7801,7 +7813,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>25</v>
@@ -7824,7 +7836,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>25</v>
@@ -7847,7 +7859,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>25</v>
@@ -7870,7 +7882,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>25</v>
@@ -7893,7 +7905,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>25</v>
@@ -7916,7 +7928,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>25</v>
@@ -7939,7 +7951,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>25</v>
@@ -7962,7 +7974,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>25</v>
@@ -7985,7 +7997,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -8004,7 +8016,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>25</v>
@@ -8025,7 +8037,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>25</v>
@@ -8048,7 +8060,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>25</v>
@@ -8073,7 +8085,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>25</v>
@@ -8096,7 +8108,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>25</v>
@@ -8119,7 +8131,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>25</v>
@@ -8142,7 +8154,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>25</v>
@@ -8165,7 +8177,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>25</v>
@@ -8188,7 +8200,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>25</v>
@@ -8211,7 +8223,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>25</v>
@@ -8234,7 +8246,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>25</v>
@@ -8257,7 +8269,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>25</v>
@@ -8280,7 +8292,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15">
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>25</v>
@@ -8303,7 +8315,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -8322,7 +8334,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>25</v>
@@ -8345,7 +8357,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>25</v>
@@ -8368,7 +8380,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>25</v>
@@ -8391,7 +8403,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>25</v>
@@ -8414,7 +8426,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15">
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>25</v>
@@ -8437,7 +8449,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15">
+    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>25</v>
@@ -8460,7 +8472,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>25</v>
@@ -8483,7 +8495,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15">
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>25</v>
@@ -8506,7 +8518,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15">
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>25</v>
@@ -8529,7 +8541,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15">
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>25</v>
@@ -8552,7 +8564,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -8571,7 +8583,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15">
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>25</v>
@@ -8596,7 +8608,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15">
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8615,7 +8627,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15">
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>25</v>
@@ -8636,7 +8648,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="15">
+    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>25</v>
@@ -8661,7 +8673,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15">
+    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8680,7 +8692,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15">
+    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>25</v>
@@ -8703,7 +8715,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15">
+    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>25</v>
@@ -8728,7 +8740,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15">
+    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>25</v>
@@ -8751,7 +8763,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>25</v>
@@ -8772,7 +8784,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15">
+    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8791,7 +8803,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15">
+    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>25</v>
@@ -8816,7 +8828,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15">
+    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>25</v>
@@ -8839,7 +8851,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15">
+    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>25</v>
@@ -8862,7 +8874,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>25</v>
@@ -8885,7 +8897,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15">
+    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>25</v>
@@ -8908,7 +8920,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>25</v>
@@ -8931,7 +8943,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>25</v>
@@ -8954,7 +8966,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -8973,7 +8985,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>25</v>
@@ -8996,7 +9008,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>25</v>
@@ -9019,7 +9031,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>25</v>
@@ -9042,7 +9054,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -9061,7 +9073,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>25</v>
@@ -9084,7 +9096,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>25</v>
@@ -9107,7 +9119,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15">
+    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>25</v>
@@ -9130,7 +9142,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15">
+    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>25</v>
@@ -9153,7 +9165,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15">
+    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>25</v>
@@ -9176,7 +9188,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15">
+    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>25</v>
@@ -9199,7 +9211,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15">
+    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -9218,7 +9230,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>25</v>
@@ -9243,7 +9255,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15">
+    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>25</v>
@@ -9266,7 +9278,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15">
+    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>25</v>
@@ -9289,7 +9301,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>25</v>
@@ -9312,7 +9324,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>25</v>
@@ -9335,7 +9347,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15">
+    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>25</v>
@@ -9358,7 +9370,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15">
+    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>25</v>
@@ -9381,7 +9393,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15">
+    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>25</v>
@@ -9404,7 +9416,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15">
+    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>25</v>
@@ -9427,7 +9439,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15">
+    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -9446,7 +9458,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15">
+    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>25</v>
@@ -9471,7 +9483,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15">
+    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>25</v>
@@ -9492,7 +9504,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15">
+    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>25</v>
@@ -9515,7 +9527,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15">
+    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>25</v>
@@ -9538,7 +9550,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15">
+    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>25</v>
@@ -9561,7 +9573,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15">
+    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>25</v>
@@ -9584,7 +9596,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15">
+    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>25</v>
@@ -9607,7 +9619,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15">
+    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>25</v>
@@ -9630,7 +9642,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15">
+    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>25</v>
@@ -9653,7 +9665,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15">
+    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>25</v>
@@ -9676,7 +9688,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15">
+    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>25</v>
@@ -9699,7 +9711,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15">
+    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>25</v>
@@ -9722,7 +9734,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15">
+    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>25</v>
@@ -9745,7 +9757,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15">
+    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>25</v>
@@ -9768,7 +9780,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15">
+    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9787,7 +9799,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15">
+    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>25</v>
@@ -9810,7 +9822,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15">
+    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9829,7 +9841,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15">
+    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>25</v>
@@ -9852,7 +9864,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15">
+    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>25</v>
@@ -9875,7 +9887,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9894,7 +9906,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15">
+    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>25</v>
@@ -9919,7 +9931,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15">
+    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>25</v>
@@ -9942,7 +9954,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15">
+    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>25</v>
@@ -9965,7 +9977,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15">
+    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>25</v>
@@ -9988,7 +10000,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15">
+    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>25</v>
@@ -10011,7 +10023,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15">
+    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>25</v>
@@ -10034,7 +10046,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15">
+    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>25</v>
@@ -10057,7 +10069,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15">
+    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>25</v>
@@ -10080,7 +10092,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15">
+    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>25</v>
@@ -10103,7 +10115,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15">
+    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>25</v>
@@ -10126,7 +10138,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15">
+    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -10145,7 +10157,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15">
+    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>25</v>
@@ -10170,7 +10182,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15">
+    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>25</v>
@@ -10193,7 +10205,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15">
+    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>25</v>
@@ -10216,7 +10228,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15">
+    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>25</v>
@@ -10239,7 +10251,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15">
+    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>25</v>
@@ -10262,7 +10274,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15">
+    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>25</v>
@@ -10285,7 +10297,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15">
+    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>25</v>
@@ -10308,7 +10320,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15">
+    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>25</v>
@@ -10331,7 +10343,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15">
+    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>25</v>
@@ -10354,7 +10366,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15">
+    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>25</v>
@@ -10377,7 +10389,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15">
+    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -10396,7 +10408,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15">
+    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>25</v>
@@ -10419,7 +10431,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15">
+    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>25</v>
@@ -10442,7 +10454,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15">
+    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>25</v>
@@ -10465,7 +10477,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15">
+    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>25</v>
@@ -10488,7 +10500,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15">
+    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -10507,7 +10519,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15">
+    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>25</v>
@@ -10530,7 +10542,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15">
+    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>25</v>
@@ -10553,7 +10565,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15">
+    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>25</v>
@@ -10576,7 +10588,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15">
+    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>25</v>
@@ -10599,7 +10611,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15">
+    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10618,7 +10630,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15">
+    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>25</v>
@@ -10639,7 +10651,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15">
+    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>25</v>
@@ -10662,7 +10674,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15">
+    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10681,7 +10693,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15">
+    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>25</v>
@@ -10704,7 +10716,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15">
+    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>25</v>
@@ -10729,7 +10741,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15">
+    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>25</v>
@@ -10750,7 +10762,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15">
+    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>25</v>
@@ -10775,7 +10787,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15">
+    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>25</v>
@@ -10800,7 +10812,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15">
+    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10819,7 +10831,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15">
+    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>25</v>
@@ -10844,7 +10856,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15">
+    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>25</v>
@@ -10867,7 +10879,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15">
+    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>25</v>
@@ -10890,7 +10902,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15">
+    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>25</v>
@@ -10913,7 +10925,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15">
+    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>25</v>
@@ -10936,7 +10948,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15">
+    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>25</v>
@@ -10959,7 +10971,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15">
+    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>25</v>
@@ -10982,7 +10994,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15">
+    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>25</v>
@@ -11005,7 +11017,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15">
+    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>25</v>
@@ -11028,7 +11040,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15">
+    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -11047,7 +11059,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15">
+    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>25</v>
@@ -11072,7 +11084,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15">
+    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>25</v>
@@ -11095,7 +11107,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15">
+    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>25</v>
@@ -11118,7 +11130,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15">
+    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>25</v>
@@ -11141,7 +11153,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15">
+    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>25</v>
@@ -11164,7 +11176,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15">
+    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>25</v>
@@ -11187,7 +11199,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15">
+    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>25</v>
@@ -11210,7 +11222,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15">
+    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>25</v>
@@ -11233,7 +11245,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15">
+    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>25</v>
@@ -11256,7 +11268,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15">
+    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -11275,7 +11287,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15">
+    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>25</v>
@@ -11296,7 +11308,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15">
+    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>25</v>
@@ -11319,7 +11331,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15">
+    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>25</v>
@@ -11342,7 +11354,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15">
+    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>25</v>
@@ -11365,7 +11377,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15">
+    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>25</v>
@@ -11388,7 +11400,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15">
+    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>25</v>
@@ -11411,7 +11423,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15">
+    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>25</v>
@@ -11434,7 +11446,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15">
+    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>25</v>
@@ -11457,7 +11469,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15">
+    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>25</v>
@@ -11480,7 +11492,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15">
+    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>25</v>
@@ -11503,7 +11515,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15">
+    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>25</v>
@@ -11526,7 +11538,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15">
+    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>25</v>
@@ -11549,7 +11561,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15">
+    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>25</v>
@@ -11572,7 +11584,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15">
+    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>25</v>
@@ -11595,7 +11607,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15">
+    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>25</v>
@@ -11618,7 +11630,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15">
+    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>25</v>
@@ -11641,7 +11653,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15">
+    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11660,7 +11672,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15">
+    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>25</v>
@@ -11681,7 +11693,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15">
+    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>25</v>
@@ -11704,7 +11716,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15">
+    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>25</v>
@@ -11727,7 +11739,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15">
+    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>25</v>
@@ -11750,7 +11762,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15">
+    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>25</v>
@@ -11773,7 +11785,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15">
+    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>25</v>
@@ -11796,7 +11808,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15">
+    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>25</v>
@@ -11819,7 +11831,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15">
+    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>25</v>
@@ -11842,7 +11854,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15">
+    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>25</v>
@@ -11865,7 +11877,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15">
+    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>25</v>
@@ -11888,7 +11900,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15">
+    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>25</v>
@@ -11911,7 +11923,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15">
+    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>25</v>
@@ -11934,7 +11946,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15">
+    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>25</v>
@@ -11957,7 +11969,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15">
+    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>25</v>
@@ -11980,7 +11992,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15">
+    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>25</v>
@@ -12003,7 +12015,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15">
+    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>25</v>
@@ -12026,7 +12038,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15">
+    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -12045,7 +12057,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15">
+    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>25</v>
@@ -12070,7 +12082,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15">
+    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>25</v>
@@ -12093,7 +12105,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15">
+    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>25</v>
@@ -12116,7 +12128,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15">
+    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>25</v>
@@ -12139,7 +12151,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15">
+    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>25</v>
@@ -12162,7 +12174,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15">
+    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -12181,7 +12193,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15">
+    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>25</v>
@@ -12206,7 +12218,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15">
+    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>25</v>
@@ -12229,7 +12241,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15">
+    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -12248,7 +12260,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15">
+    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -12267,7 +12279,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15">
+    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -12286,7 +12298,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15">
+    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>25</v>
@@ -12307,7 +12319,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15">
+    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>25</v>
@@ -12330,7 +12342,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15">
+    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>25</v>
@@ -12353,7 +12365,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15">
+    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>25</v>
@@ -12376,7 +12388,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15">
+    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>25</v>
@@ -12399,7 +12411,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15">
+    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>25</v>
@@ -12422,7 +12434,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15">
+    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>25</v>
@@ -12445,7 +12457,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15">
+    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>25</v>
@@ -12468,7 +12480,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15">
+    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>25</v>
@@ -12491,7 +12503,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15">
+    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>25</v>
@@ -12514,7 +12526,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15">
+    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>25</v>
@@ -12537,7 +12549,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15">
+    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -12556,7 +12568,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15">
+    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>25</v>
@@ -12579,7 +12591,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15">
+    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -12598,7 +12610,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15">
+    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>25</v>
@@ -12623,7 +12635,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15">
+    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>25</v>
@@ -12646,7 +12658,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15">
+    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>25</v>
@@ -12669,7 +12681,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15">
+    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>25</v>
@@ -12692,7 +12704,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15">
+    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>25</v>
@@ -12715,7 +12727,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15">
+    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>25</v>
@@ -12738,7 +12750,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15">
+    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>25</v>
@@ -12761,7 +12773,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15">
+    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>25</v>
@@ -12784,7 +12796,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15">
+    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>25</v>
@@ -12807,7 +12819,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15">
+    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>25</v>
@@ -12830,7 +12842,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15">
+    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>25</v>
@@ -12853,7 +12865,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15">
+    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12872,7 +12884,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15">
+    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>25</v>
@@ -12895,7 +12907,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15">
+    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12914,7 +12926,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15">
+    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>25</v>
@@ -12935,7 +12947,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15">
+    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -12954,7 +12966,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15">
+    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>25</v>
@@ -12975,7 +12987,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15">
+    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -12994,7 +13006,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15">
+    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>25</v>
@@ -13015,7 +13027,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15">
+    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -13034,7 +13046,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15">
+    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>25</v>
@@ -13057,7 +13069,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15">
+    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -13076,7 +13088,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15">
+    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>25</v>
@@ -13101,7 +13113,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15">
+    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>25</v>
@@ -13124,7 +13136,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15">
+    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>25</v>
@@ -13147,7 +13159,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15">
+    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>25</v>
@@ -13170,7 +13182,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15">
+    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>25</v>
@@ -13193,7 +13205,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15">
+    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>25</v>
@@ -13216,7 +13228,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15">
+    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>25</v>
@@ -13239,7 +13251,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15">
+    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>25</v>
@@ -13262,7 +13274,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15">
+    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>25</v>
@@ -13285,7 +13297,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15">
+    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -13304,7 +13316,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15">
+    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>25</v>
@@ -13327,7 +13339,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15">
+    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>25</v>
@@ -13350,7 +13362,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15">
+    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>25</v>
@@ -13373,7 +13385,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15">
+    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>25</v>
@@ -13396,7 +13408,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15">
+    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -13415,7 +13427,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15">
+    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>25</v>
@@ -13438,7 +13450,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15">
+    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>25</v>
@@ -13461,7 +13473,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15">
+    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>25</v>
@@ -13486,7 +13498,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15">
+    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -13505,7 +13517,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15">
+    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>25</v>
@@ -13530,7 +13542,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15">
+    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>25</v>
@@ -13553,7 +13565,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15">
+    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -13572,7 +13584,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15">
+    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>25</v>
@@ -13593,7 +13605,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15">
+    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>25</v>
@@ -13614,7 +13626,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15">
+    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>25</v>
@@ -13637,7 +13649,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15">
+    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13656,7 +13668,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15">
+    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13675,7 +13687,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15">
+    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>25</v>
@@ -13700,7 +13712,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15">
+    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>25</v>
@@ -13743,13 +13755,13 @@
       <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>465</v>
       </c>
@@ -13760,7 +13772,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>455</v>
       </c>
@@ -13771,7 +13783,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>456</v>
       </c>
@@ -13782,7 +13794,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>463</v>
       </c>
@@ -13793,7 +13805,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>457</v>
       </c>
@@ -13804,17 +13816,17 @@
         <v>462</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
cleanup all projects and move to 2.0
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19700" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="652">
   <si>
     <t>type</t>
   </si>
@@ -1498,9 +1498,6 @@
     <t>OpenStudio Server Version</t>
   </si>
   <si>
-    <t>Choose which OpenStudio Server Version to Use.  Do NOT change this unless advised.</t>
-  </si>
-  <si>
     <t>Cluster Name</t>
   </si>
   <si>
@@ -1762,9 +1759,6 @@
     <t>0.2.0</t>
   </si>
   <si>
-    <t>1.3.1</t>
-  </si>
-  <si>
     <t>AnalysisType</t>
   </si>
   <si>
@@ -1903,81 +1897,6 @@
     <t>Total Natural Gas</t>
   </si>
   <si>
-    <t>cooling_electricity_jan</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>cooling_electricity_feb</t>
-  </si>
-  <si>
-    <t>cooling_electricity_mar</t>
-  </si>
-  <si>
-    <t>cooling_electricity_apr</t>
-  </si>
-  <si>
-    <t>cooling_electricity_may</t>
-  </si>
-  <si>
-    <t>cooling_electricity_jun</t>
-  </si>
-  <si>
-    <t>cooling_electricity_jul</t>
-  </si>
-  <si>
-    <t>cooling_electricity_aug</t>
-  </si>
-  <si>
-    <t>cooling_electricity_sep</t>
-  </si>
-  <si>
-    <t>cooling_electricity_oct</t>
-  </si>
-  <si>
-    <t>cooling_electricity_nov</t>
-  </si>
-  <si>
-    <t>cooling_electricity_dec</t>
-  </si>
-  <si>
-    <t>heating_gas_jan</t>
-  </si>
-  <si>
-    <t>heating_gas_feb</t>
-  </si>
-  <si>
-    <t>heating_gas_mar</t>
-  </si>
-  <si>
-    <t>heating_gas_apr</t>
-  </si>
-  <si>
-    <t>heating_gas_may</t>
-  </si>
-  <si>
-    <t>heating_gas_jun</t>
-  </si>
-  <si>
-    <t>heating_gas_jul</t>
-  </si>
-  <si>
-    <t>heating_gas_aug</t>
-  </si>
-  <si>
-    <t>heating_gas_sep</t>
-  </si>
-  <si>
-    <t>heating_gas_oct</t>
-  </si>
-  <si>
-    <t>heating_gas_nov</t>
-  </si>
-  <si>
-    <t>heating_gas_dec</t>
-  </si>
-  <si>
     <t>m3.large</t>
   </si>
   <si>
@@ -2023,9 +1942,6 @@
     <t>c3.8xlarge</t>
   </si>
   <si>
-    <t>32 Cores</t>
-  </si>
-  <si>
     <t>$1.68/hour</t>
   </si>
   <si>
@@ -2035,9 +1951,6 @@
     <t xml:space="preserve"> - Worker Only - Recommended for Worker</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Worker Only</t>
-  </si>
-  <si>
     <t>Number of worker nodes to start.</t>
   </si>
   <si>
@@ -2063,6 +1976,27 @@
   </si>
   <si>
     <t>If extra library files are needed then include them here. These are typically preprocessors or postprocessors and require custom measures to use.</t>
+  </si>
+  <si>
+    <t>Choose which OpenStudio Server Version to Use.  Do NOT change this unless advised. Note that this is not the OpenStudio version.  See mappings here: http://developer.nrel.gov/downloads/buildings/openstudio/rsrc/amis_v2.json</t>
+  </si>
+  <si>
+    <t>1.5.6</t>
+  </si>
+  <si>
+    <t>Total Site Energy</t>
+  </si>
+  <si>
+    <t>total_energy</t>
+  </si>
+  <si>
+    <t>Total Source Energy</t>
+  </si>
+  <si>
+    <t>total_source_energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Worker Only - </t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2063,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2184,18 +2118,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF1DE"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2206,7 +2128,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1421">
+  <cellStyleXfs count="1439">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3628,8 +3550,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3711,25 +3651,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1421">
+  <cellStyles count="1439">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4440,6 +4378,15 @@
     <cellStyle name="Followed Hyperlink" xfId="1416" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1418" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1438" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5150,6 +5097,15 @@
     <cellStyle name="Hyperlink" xfId="1415" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1417" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1437" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5451,7 +5407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5485,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5495,7 +5451,7 @@
     <col min="2" max="2" width="30.33203125" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -5522,7 +5478,7 @@
         <v>443</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>444</v>
@@ -5533,32 +5489,32 @@
         <v>467</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28">
+    <row r="5" spans="1:5" ht="56">
       <c r="A5" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>573</v>
+      <c r="B5" s="32" t="s">
+        <v>646</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>485</v>
+        <v>645</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="46" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>662</v>
+        <v>634</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5566,18 +5522,18 @@
         <v>449</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>645</v>
-      </c>
-      <c r="C7" s="44" t="str">
+        <v>618</v>
+      </c>
+      <c r="C7" s="41" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
         <v>2 Cores - Recommended for Server</v>
       </c>
-      <c r="D7" s="44" t="str">
+      <c r="D7" s="41" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
         <v>$0.14/hour</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>666</v>
+        <v>637</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28">
@@ -5587,11 +5543,11 @@
       <c r="B8" s="31" t="s">
         <v>447</v>
       </c>
-      <c r="C8" s="44" t="str">
+      <c r="C8" s="41" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
         <v>8 Cores - Worker Only - Recommended for Worker</v>
       </c>
-      <c r="D8" s="44" t="str">
+      <c r="D8" s="41" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
         <v>$0.42/hour</v>
       </c>
@@ -5607,9 +5563,9 @@
         <v>1</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="44"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="2" t="s">
-        <v>665</v>
+        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="13" customFormat="1">
@@ -5626,10 +5582,10 @@
         <v>43</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5640,7 +5596,7 @@
         <v>460</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5662,7 +5618,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>478</v>
       </c>
@@ -5670,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>667</v>
+        <v>638</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5689,18 +5645,18 @@
         <v>481</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A20" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>668</v>
+        <v>639</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -5720,18 +5676,18 @@
       <c r="B22" s="32"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A23" s="12" t="s">
         <v>458</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>671</v>
+        <v>642</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>669</v>
+        <v>640</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>466</v>
@@ -5746,11 +5702,11 @@
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v>individual_variables</v>
       </c>
-      <c r="C24" s="46" t="str">
+      <c r="C24" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,1,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>individual_variables / all_variables</v>
       </c>
-      <c r="D24" s="47"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="1:5" ht="42">
       <c r="A25" s="37" t="str">
@@ -5761,11 +5717,11 @@
         <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v>30</v>
       </c>
-      <c r="C25" s="46" t="str">
+      <c r="C25" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,2,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="43"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="37" t="str">
@@ -5776,11 +5732,11 @@
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C26" s="46" t="str">
+      <c r="C26" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,3,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:5" s="37" customFormat="1">
       <c r="A27" s="37" t="str">
@@ -5791,11 +5747,11 @@
         <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C27" s="46" t="str">
+      <c r="C27" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,4,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="1:5" s="37" customFormat="1">
       <c r="A28" s="37" t="str">
@@ -5806,11 +5762,11 @@
         <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C28" s="46" t="str">
+      <c r="C28" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,5,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="1:5" s="37" customFormat="1">
       <c r="A29" s="37" t="str">
@@ -5821,11 +5777,11 @@
         <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C29" s="46" t="str">
+      <c r="C29" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,6,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="1:5" s="37" customFormat="1">
       <c r="A30" s="37" t="str">
@@ -5836,11 +5792,11 @@
         <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C30" s="46" t="str">
+      <c r="C30" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,7,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="43"/>
     </row>
     <row r="31" spans="1:5" s="37" customFormat="1">
       <c r="A31" s="37" t="str">
@@ -5851,11 +5807,11 @@
         <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C31" s="46" t="str">
+      <c r="C31" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,8,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D31" s="47"/>
+      <c r="D31" s="43"/>
     </row>
     <row r="32" spans="1:5" s="37" customFormat="1">
       <c r="A32" s="37" t="str">
@@ -5866,11 +5822,11 @@
         <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C32" s="46" t="str">
+      <c r="C32" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,9,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D32" s="47"/>
+      <c r="D32" s="43"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="37" t="str">
@@ -5881,11 +5837,11 @@
         <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C33" s="46" t="str">
+      <c r="C33" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$26,10,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D33" s="47"/>
+      <c r="D33" s="43"/>
     </row>
     <row r="34" spans="1:5" s="37" customFormat="1">
       <c r="A34" s="37" t="str">
@@ -5896,11 +5852,11 @@
         <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)-1)))</f>
         <v/>
       </c>
-      <c r="C34" s="46" t="str">
+      <c r="C34" s="42" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))=0,"",INDEX(Lookups!$C$17:$Z$27,11,3*MATCH(Setup!$B21,Lookups!$A$17:$A$23,0)))</f>
         <v/>
       </c>
-      <c r="D34" s="47"/>
+      <c r="D34" s="43"/>
     </row>
     <row r="35" spans="1:5" s="37" customFormat="1">
       <c r="B35" s="32"/>
@@ -5920,11 +5876,11 @@
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="29" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="44" t="s">
         <v>459</v>
       </c>
     </row>
@@ -5950,13 +5906,13 @@
         <v>35</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="47" t="s">
-        <v>616</v>
+      <c r="D40" s="43" t="s">
+        <v>614</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>457</v>
@@ -5970,11 +5926,11 @@
         <v>37</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>672</v>
+        <v>643</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="14" t="s">
-        <v>673</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -6052,27 +6008,27 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="25" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
       <c r="P1" s="39" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
@@ -6082,10 +6038,10 @@
         <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -6134,13 +6090,13 @@
         <v>9</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="P3" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q3" s="18" t="s">
         <v>492</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>493</v>
       </c>
       <c r="R3" s="11" t="s">
         <v>8</v>
@@ -7114,13 +7070,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>73</v>
@@ -7131,10 +7087,10 @@
         <v>24</v>
       </c>
       <c r="D37" s="36" t="s">
+        <v>549</v>
+      </c>
+      <c r="E37" s="36" t="s">
         <v>550</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>551</v>
       </c>
       <c r="F37" s="36" t="s">
         <v>15</v>
@@ -7170,13 +7126,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E38" s="37" t="s">
         <v>73</v>
@@ -7187,10 +7143,10 @@
         <v>24</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F39" s="36" t="s">
         <v>15</v>
@@ -8155,7 +8111,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8197,10 +8153,10 @@
         <v>474</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="16" customFormat="1" ht="30">
@@ -8214,543 +8170,238 @@
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="37" customFormat="1">
-      <c r="A4" s="36" t="s">
-        <v>619</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>556</v>
-      </c>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="28" t="s">
+        <v>617</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>483</v>
       </c>
-      <c r="D4" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="38">
-        <v>140</v>
-      </c>
+      <c r="D4" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="38"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" s="37" customFormat="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="28" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>557</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>558</v>
-      </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="28" t="s">
         <v>483</v>
       </c>
-      <c r="D5" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="38">
-        <v>590</v>
-      </c>
+      <c r="D5" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="38"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>620</v>
-      </c>
-      <c r="B6" t="s">
-        <v>620</v>
-      </c>
-      <c r="C6" t="s">
-        <v>621</v>
-      </c>
-      <c r="D6" t="b">
+      <c r="A6" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D6" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
-        <v>63597914341</v>
-      </c>
-      <c r="F6" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="F6" s="35"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>622</v>
-      </c>
-      <c r="B7" t="s">
-        <v>622</v>
-      </c>
-      <c r="C7" t="s">
-        <v>621</v>
-      </c>
-      <c r="D7" t="b">
+      <c r="A7" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D7" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>58138465958</v>
-      </c>
-      <c r="F7" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="F7" s="35"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>623</v>
-      </c>
-      <c r="B8" t="s">
-        <v>623</v>
-      </c>
-      <c r="C8" t="s">
-        <v>621</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="40">
-        <v>301532000000</v>
-      </c>
-      <c r="F8" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="35"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>624</v>
-      </c>
-      <c r="B9" t="s">
-        <v>624</v>
-      </c>
-      <c r="C9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="40">
-        <v>336163000000</v>
-      </c>
-      <c r="F9" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="35"/>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>625</v>
-      </c>
-      <c r="B10" t="s">
-        <v>625</v>
-      </c>
-      <c r="C10" t="s">
-        <v>621</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="40">
-        <v>1412750000000</v>
-      </c>
-      <c r="F10" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="35"/>
       <c r="G10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>626</v>
-      </c>
-      <c r="B11" t="s">
-        <v>626</v>
-      </c>
-      <c r="C11" t="s">
-        <v>621</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="40">
-        <v>2327740000000</v>
-      </c>
-      <c r="F11" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="35"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>627</v>
-      </c>
-      <c r="B12" t="s">
-        <v>627</v>
-      </c>
-      <c r="C12" t="s">
-        <v>621</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="40">
-        <v>2402590000000</v>
-      </c>
-      <c r="F12" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="35"/>
       <c r="G12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>628</v>
-      </c>
-      <c r="B13" t="s">
-        <v>628</v>
-      </c>
-      <c r="C13" t="s">
-        <v>621</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="40">
-        <v>2472660000000</v>
-      </c>
-      <c r="F13" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="35"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>629</v>
-      </c>
-      <c r="B14" t="s">
-        <v>629</v>
-      </c>
-      <c r="C14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="40">
-        <v>1807430000000</v>
-      </c>
-      <c r="F14" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="35"/>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:7" customFormat="1">
-      <c r="A15" t="s">
-        <v>630</v>
-      </c>
-      <c r="B15" t="s">
-        <v>630</v>
-      </c>
-      <c r="C15" t="s">
-        <v>621</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="40">
-        <v>619616000000</v>
-      </c>
-      <c r="F15" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:7" customFormat="1">
-      <c r="A16" t="s">
-        <v>631</v>
-      </c>
-      <c r="B16" t="s">
-        <v>631</v>
-      </c>
-      <c r="C16" t="s">
-        <v>621</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="40">
-        <v>117110000000</v>
-      </c>
-      <c r="F16" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:7" customFormat="1">
-      <c r="A17" t="s">
-        <v>632</v>
-      </c>
-      <c r="B17" t="s">
-        <v>632</v>
-      </c>
-      <c r="C17" t="s">
-        <v>621</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="35">
-        <v>103360000000</v>
-      </c>
-      <c r="F17" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:7" customFormat="1">
-      <c r="A18" t="s">
-        <v>633</v>
-      </c>
-      <c r="B18" t="s">
-        <v>633</v>
-      </c>
-      <c r="C18" t="s">
-        <v>621</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="40">
-        <v>2799560000000</v>
-      </c>
-      <c r="F18" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:7" customFormat="1">
-      <c r="A19" t="s">
-        <v>634</v>
-      </c>
-      <c r="B19" t="s">
-        <v>634</v>
-      </c>
-      <c r="C19" t="s">
-        <v>621</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="40">
-        <v>2663350000000</v>
-      </c>
-      <c r="F19" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="1:7" customFormat="1">
-      <c r="A20" t="s">
-        <v>635</v>
-      </c>
-      <c r="B20" t="s">
-        <v>635</v>
-      </c>
-      <c r="C20" t="s">
-        <v>621</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="40">
-        <v>1576140000000</v>
-      </c>
-      <c r="F20" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>636</v>
-      </c>
-      <c r="B21" t="s">
-        <v>636</v>
-      </c>
-      <c r="C21" t="s">
-        <v>621</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="40">
-        <v>1752790000000</v>
-      </c>
-      <c r="F21" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="35"/>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>637</v>
-      </c>
-      <c r="B22" t="s">
-        <v>637</v>
-      </c>
-      <c r="C22" t="s">
-        <v>621</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="40">
-        <v>375145000000</v>
-      </c>
-      <c r="F22" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="35"/>
       <c r="G22"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>638</v>
-      </c>
-      <c r="B23" t="s">
-        <v>638</v>
-      </c>
-      <c r="C23" t="s">
-        <v>621</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>32970706746</v>
-      </c>
-      <c r="F23" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="F23" s="35"/>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>639</v>
-      </c>
-      <c r="B24" t="s">
-        <v>639</v>
-      </c>
-      <c r="C24" t="s">
-        <v>621</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>50096876833</v>
-      </c>
-      <c r="F24" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="F24" s="35"/>
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>640</v>
-      </c>
-      <c r="B25" t="s">
-        <v>640</v>
-      </c>
-      <c r="C25" t="s">
-        <v>621</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>32660740138</v>
-      </c>
-      <c r="F25" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="F25" s="35"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>641</v>
-      </c>
-      <c r="B26" t="s">
-        <v>641</v>
-      </c>
-      <c r="C26" t="s">
-        <v>621</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="40">
-        <v>144098000000</v>
-      </c>
-      <c r="F26" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="35"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>642</v>
-      </c>
-      <c r="B27" t="s">
-        <v>642</v>
-      </c>
-      <c r="C27" t="s">
-        <v>621</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="40">
-        <v>970976000000</v>
-      </c>
-      <c r="F27" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="35"/>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B28" t="s">
-        <v>643</v>
-      </c>
-      <c r="C28" t="s">
-        <v>621</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="40">
-        <v>2261120000000</v>
-      </c>
-      <c r="F28" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="35"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>644</v>
-      </c>
-      <c r="B29" t="s">
-        <v>644</v>
-      </c>
-      <c r="C29" t="s">
-        <v>621</v>
-      </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="35">
-        <v>2657740000000</v>
-      </c>
-      <c r="F29" s="35">
-        <v>463204000000</v>
-      </c>
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7">
@@ -16133,10 +15784,10 @@
         <v>0</v>
       </c>
       <c r="B328" t="s">
+        <v>493</v>
+      </c>
+      <c r="C328" t="s">
         <v>494</v>
-      </c>
-      <c r="C328" t="s">
-        <v>495</v>
       </c>
       <c r="D328" t="s">
         <v>73</v>
@@ -16147,10 +15798,10 @@
         <v>23</v>
       </c>
       <c r="C329" t="s">
+        <v>495</v>
+      </c>
+      <c r="D329" t="s">
         <v>496</v>
-      </c>
-      <c r="D329" t="s">
-        <v>497</v>
       </c>
       <c r="E329" t="s">
         <v>2</v>
@@ -16159,10 +15810,10 @@
         <v>67</v>
       </c>
       <c r="H329" t="s">
+        <v>497</v>
+      </c>
+      <c r="I329" t="s">
         <v>498</v>
-      </c>
-      <c r="I329" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="330" spans="1:9">
@@ -16170,10 +15821,10 @@
         <v>23</v>
       </c>
       <c r="C330" t="s">
+        <v>499</v>
+      </c>
+      <c r="D330" t="s">
         <v>500</v>
-      </c>
-      <c r="D330" t="s">
-        <v>501</v>
       </c>
       <c r="E330" t="s">
         <v>2</v>
@@ -16190,10 +15841,10 @@
         <v>23</v>
       </c>
       <c r="C331" t="s">
+        <v>501</v>
+      </c>
+      <c r="D331" t="s">
         <v>502</v>
-      </c>
-      <c r="D331" t="s">
-        <v>503</v>
       </c>
       <c r="E331" t="s">
         <v>2</v>
@@ -16210,10 +15861,10 @@
         <v>23</v>
       </c>
       <c r="C332" t="s">
+        <v>503</v>
+      </c>
+      <c r="D332" t="s">
         <v>504</v>
-      </c>
-      <c r="D332" t="s">
-        <v>505</v>
       </c>
       <c r="E332" t="s">
         <v>2</v>
@@ -16230,10 +15881,10 @@
         <v>23</v>
       </c>
       <c r="C333" t="s">
+        <v>505</v>
+      </c>
+      <c r="D333" t="s">
         <v>506</v>
-      </c>
-      <c r="D333" t="s">
-        <v>507</v>
       </c>
       <c r="E333" t="s">
         <v>2</v>
@@ -16247,10 +15898,10 @@
         <v>23</v>
       </c>
       <c r="C334" t="s">
+        <v>507</v>
+      </c>
+      <c r="D334" t="s">
         <v>508</v>
-      </c>
-      <c r="D334" t="s">
-        <v>509</v>
       </c>
       <c r="E334" t="s">
         <v>2</v>
@@ -16259,10 +15910,10 @@
         <v>67</v>
       </c>
       <c r="H334" t="s">
+        <v>509</v>
+      </c>
+      <c r="I334" t="s">
         <v>510</v>
-      </c>
-      <c r="I334" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="335" spans="1:9">
@@ -16270,10 +15921,10 @@
         <v>23</v>
       </c>
       <c r="C335" t="s">
+        <v>511</v>
+      </c>
+      <c r="D335" t="s">
         <v>512</v>
-      </c>
-      <c r="D335" t="s">
-        <v>513</v>
       </c>
       <c r="E335" t="s">
         <v>2</v>
@@ -16282,10 +15933,10 @@
         <v>67</v>
       </c>
       <c r="H335" t="s">
+        <v>513</v>
+      </c>
+      <c r="I335" t="s">
         <v>514</v>
-      </c>
-      <c r="I335" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="336" spans="1:9">
@@ -16293,10 +15944,10 @@
         <v>0</v>
       </c>
       <c r="B336" t="s">
+        <v>515</v>
+      </c>
+      <c r="C336" t="s">
         <v>516</v>
-      </c>
-      <c r="C336" t="s">
-        <v>517</v>
       </c>
       <c r="D336" t="s">
         <v>73</v>
@@ -16307,10 +15958,10 @@
         <v>23</v>
       </c>
       <c r="C337" t="s">
+        <v>517</v>
+      </c>
+      <c r="D337" t="s">
         <v>518</v>
-      </c>
-      <c r="D337" t="s">
-        <v>519</v>
       </c>
       <c r="E337" t="s">
         <v>2</v>
@@ -16319,10 +15970,10 @@
         <v>67</v>
       </c>
       <c r="H337" t="s">
+        <v>519</v>
+      </c>
+      <c r="I337" t="s">
         <v>520</v>
-      </c>
-      <c r="I337" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="338" spans="1:16">
@@ -16330,10 +15981,10 @@
         <v>23</v>
       </c>
       <c r="C338" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D338" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E338" t="s">
         <v>2</v>
@@ -16342,10 +15993,10 @@
         <v>67</v>
       </c>
       <c r="H338" t="s">
+        <v>522</v>
+      </c>
+      <c r="I338" t="s">
         <v>523</v>
-      </c>
-      <c r="I338" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="339" spans="1:16">
@@ -16353,10 +16004,10 @@
         <v>23</v>
       </c>
       <c r="C339" t="s">
+        <v>524</v>
+      </c>
+      <c r="D339" t="s">
         <v>525</v>
-      </c>
-      <c r="D339" t="s">
-        <v>526</v>
       </c>
       <c r="E339" t="s">
         <v>2</v>
@@ -16373,10 +16024,10 @@
         <v>23</v>
       </c>
       <c r="C340" t="s">
+        <v>526</v>
+      </c>
+      <c r="D340" t="s">
         <v>527</v>
-      </c>
-      <c r="D340" t="s">
-        <v>528</v>
       </c>
       <c r="E340" t="s">
         <v>2</v>
@@ -16393,10 +16044,10 @@
         <v>23</v>
       </c>
       <c r="C341" t="s">
+        <v>528</v>
+      </c>
+      <c r="D341" t="s">
         <v>529</v>
-      </c>
-      <c r="D341" t="s">
-        <v>530</v>
       </c>
       <c r="E341" t="s">
         <v>2</v>
@@ -16410,10 +16061,10 @@
         <v>0</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>73</v>
@@ -16437,10 +16088,10 @@
         <v>23</v>
       </c>
       <c r="C343" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D343" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E343" t="s">
         <v>2</v>
@@ -16449,10 +16100,10 @@
         <v>67</v>
       </c>
       <c r="H343" t="s">
+        <v>535</v>
+      </c>
+      <c r="I343" t="s">
         <v>536</v>
-      </c>
-      <c r="I343" t="s">
-        <v>537</v>
       </c>
       <c r="L343" s="1"/>
       <c r="M343" s="1"/>
@@ -16466,10 +16117,10 @@
         <v>23</v>
       </c>
       <c r="C344" t="s">
+        <v>533</v>
+      </c>
+      <c r="D344" t="s">
         <v>534</v>
-      </c>
-      <c r="D344" t="s">
-        <v>535</v>
       </c>
       <c r="E344" t="s">
         <v>2</v>
@@ -16504,10 +16155,10 @@
         <v>0</v>
       </c>
       <c r="B345" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C345" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D345" s="1" t="s">
         <v>73</v>
@@ -16518,10 +16169,10 @@
         <v>23</v>
       </c>
       <c r="C346" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E346" t="s">
         <v>2</v>
@@ -16732,10 +16383,10 @@
         <v>0</v>
       </c>
       <c r="B357" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C357" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D357" t="s">
         <v>73</v>
@@ -16746,10 +16397,10 @@
         <v>23</v>
       </c>
       <c r="C358" t="s">
+        <v>543</v>
+      </c>
+      <c r="D358" t="s">
         <v>544</v>
-      </c>
-      <c r="D358" t="s">
-        <v>545</v>
       </c>
       <c r="E358" t="s">
         <v>2</v>
@@ -16766,10 +16417,10 @@
         <v>23</v>
       </c>
       <c r="C359" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D359" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E359" t="s">
         <v>2</v>
@@ -16786,10 +16437,10 @@
         <v>0</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D360" s="1" t="s">
         <v>73</v>
@@ -16802,10 +16453,10 @@
         <v>23</v>
       </c>
       <c r="C361" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D361" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E361" t="s">
         <v>2</v>
@@ -16815,10 +16466,10 @@
       </c>
       <c r="G361"/>
       <c r="H361" t="s">
+        <v>535</v>
+      </c>
+      <c r="I361" t="s">
         <v>536</v>
-      </c>
-      <c r="I361" t="s">
-        <v>537</v>
       </c>
       <c r="J361"/>
       <c r="K361"/>
@@ -16829,10 +16480,10 @@
         <v>24</v>
       </c>
       <c r="C362" t="s">
+        <v>533</v>
+      </c>
+      <c r="D362" t="s">
         <v>534</v>
-      </c>
-      <c r="D362" t="s">
-        <v>535</v>
       </c>
       <c r="E362" t="s">
         <v>15</v>
@@ -16869,10 +16520,10 @@
         <v>0</v>
       </c>
       <c r="B363" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C363" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>73</v>
@@ -16883,10 +16534,10 @@
         <v>23</v>
       </c>
       <c r="C364" t="s">
+        <v>549</v>
+      </c>
+      <c r="D364" t="s">
         <v>550</v>
-      </c>
-      <c r="D364" t="s">
-        <v>551</v>
       </c>
       <c r="E364" t="s">
         <v>2</v>
@@ -16903,10 +16554,10 @@
         <v>0</v>
       </c>
       <c r="B365" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C365" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D365" s="1" t="s">
         <v>73</v>
@@ -16917,10 +16568,10 @@
         <v>23</v>
       </c>
       <c r="C366" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D366" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E366" t="s">
         <v>2</v>
@@ -16948,7 +16599,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C24"/>
+      <selection activeCell="A2" sqref="A2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16972,130 +16623,130 @@
         <v>446</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A2" s="42" t="s">
-        <v>645</v>
+    <row r="2" spans="1:21" s="36" customFormat="1">
+      <c r="A2" s="36" t="s">
+        <v>618</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>452</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>646</v>
+        <v>619</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A3" s="42" t="s">
-        <v>648</v>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="36" customFormat="1">
+      <c r="A3" s="36" t="s">
+        <v>621</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>453</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>649</v>
+        <v>622</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A4" s="42" t="s">
-        <v>650</v>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="36" customFormat="1">
+      <c r="A4" s="36" t="s">
+        <v>623</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>454</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>651</v>
+        <v>624</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A5" s="42" t="s">
-        <v>652</v>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="36" customFormat="1">
+      <c r="A5" s="36" t="s">
+        <v>625</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>452</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>653</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A6" s="42" t="s">
-        <v>654</v>
+        <v>626</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="36" customFormat="1">
+      <c r="A6" s="36" t="s">
+        <v>627</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>453</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>655</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A7" s="42" t="s">
+        <v>628</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="36" customFormat="1">
+      <c r="A7" s="36" t="s">
         <v>447</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>454</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A8" s="42" t="s">
-        <v>657</v>
+        <v>629</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="36" customFormat="1">
+      <c r="A8" s="36" t="s">
+        <v>630</v>
       </c>
       <c r="B8" s="36" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>631</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="36" customFormat="1">
+      <c r="A9" s="36" t="s">
+        <v>632</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>455</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>658</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="36" customFormat="1" ht="15">
-      <c r="A9" s="42" t="s">
-        <v>659</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>660</v>
-      </c>
       <c r="C9" s="36" t="s">
-        <v>661</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>663</v>
+        <v>633</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
+        <v>595</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>578</v>
+      </c>
+      <c r="E11" t="s">
+        <v>579</v>
+      </c>
+      <c r="G11" t="s">
         <v>597</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>580</v>
-      </c>
-      <c r="E11" t="s">
-        <v>581</v>
-      </c>
-      <c r="G11" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -17106,7 +16757,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G12" t="s">
         <v>480</v>
@@ -17120,66 +16771,66 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="36" customFormat="1"/>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C16" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L16" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="O16" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="R16" s="36" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="U16" s="36" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G17" t="s">
         <v>465</v>
       </c>
       <c r="H17" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J17" s="35">
         <v>0.01</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="M17">
         <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="O17" t="s">
         <v>4</v>
@@ -17188,7 +16839,7 @@
         <v>30</v>
       </c>
       <c r="Q17" s="36" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -17202,229 +16853,229 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="J18" s="35">
         <v>0.01</v>
       </c>
       <c r="K18" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L18" s="37" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18" s="36" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="O18" s="37" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="P18">
         <v>3</v>
       </c>
       <c r="Q18" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J19" s="35">
         <v>45036000000000</v>
       </c>
       <c r="K19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="M19">
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="O19" s="37" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P19">
         <v>0.85</v>
       </c>
       <c r="Q19" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L20" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="M20">
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="O20" s="37" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="P20">
         <v>2</v>
       </c>
       <c r="Q20" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="J21" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="J21" s="37" t="s">
-        <v>562</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="M21" s="35">
         <v>0.01</v>
       </c>
       <c r="N21" s="37" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="O21" s="37" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="P21">
         <v>2</v>
       </c>
       <c r="Q21" s="36" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J22" s="37">
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="M22" s="35">
         <v>0.01</v>
       </c>
       <c r="N22" s="37" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="O22" s="37" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="P22">
         <v>0.8</v>
       </c>
       <c r="Q22" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M23" s="35">
         <v>0.01</v>
       </c>
       <c r="N23" s="36" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="O23" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="P23" s="37" t="s">
         <v>561</v>
-      </c>
-      <c r="P23" s="37" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="L24" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="M24" s="35">
         <v>45036000000000</v>
       </c>
       <c r="N24" s="36" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="O24" s="37" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="P24" s="37">
         <v>2</v>
       </c>
       <c r="Q24" s="36" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="L25" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="M25" s="36">
         <v>100</v>
       </c>
       <c r="N25" s="36" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="L26" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="M26" s="37" t="s">
         <v>561</v>
-      </c>
-      <c r="M26" s="37" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="L27" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="M27" s="37">
         <v>2</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use new versions of gems. update template with short display names
</commit_message>
<xml_diff>
--- a/doc/template_input.xlsx
+++ b/doc/template_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16840" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -15,8 +15,8 @@
     <sheet name="Lookups" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$G$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$H$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$15</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="679">
   <si>
     <t>type</t>
   </si>
@@ -1951,18 +1951,12 @@
     <t xml:space="preserve"> - Worker Only - </t>
   </si>
   <si>
-    <t>1.6.1</t>
-  </si>
-  <si>
     <t>Template Project</t>
   </si>
   <si>
     <t>Template Model</t>
   </si>
   <si>
-    <t>0.3.0</t>
-  </si>
-  <si>
     <t>Relative to this spreadsheet or absolute path</t>
   </si>
   <si>
@@ -2048,13 +2042,49 @@
   </si>
   <si>
     <t>standard_report_legacy.total_electricity</t>
+  </si>
+  <si>
+    <t>0.3.3</t>
+  </si>
+  <si>
+    <t>1.8.0-pre2</t>
+  </si>
+  <si>
+    <t>Parameter Short Display Name</t>
+  </si>
+  <si>
+    <t>LPD Reduction</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>Wall R-Value</t>
+  </si>
+  <si>
+    <t>Roof R-Value</t>
+  </si>
+  <si>
+    <t>WWR West</t>
+  </si>
+  <si>
+    <t>Short Display Name</t>
+  </si>
+  <si>
+    <t>Short display names are used for plots and exported to metadata</t>
+  </si>
+  <si>
+    <t>Site EUI</t>
+  </si>
+  <si>
+    <t>Source EUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2111,6 +2141,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3626,7 +3661,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3716,6 +3751,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1445">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5497,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5534,7 +5574,7 @@
         <v>440</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>639</v>
+        <v>667</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>441</v>
@@ -5556,7 +5596,7 @@
         <v>476</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>636</v>
+        <v>668</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>634</v>
@@ -5638,7 +5678,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>478</v>
@@ -5652,7 +5692,7 @@
         <v>456</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5663,7 +5703,7 @@
         <v>457</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5931,7 +5971,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>33</v>
@@ -5958,7 +5998,7 @@
         <v>40</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>453</v>
@@ -5969,7 +6009,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>43</v>
@@ -5989,7 +6029,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -6026,10 +6066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y91"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6038,25 +6078,26 @@
     <col min="2" max="2" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="7.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="11.5" style="1"/>
-    <col min="17" max="17" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" style="1"/>
-    <col min="19" max="19" width="46.1640625" style="1" customWidth="1"/>
-    <col min="20" max="22" width="11.5" style="1"/>
-    <col min="23" max="23" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.5" style="1"/>
+    <col min="5" max="5" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="7.6640625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.5" style="1"/>
+    <col min="18" max="18" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="1"/>
+    <col min="20" max="20" width="46.1640625" style="1" customWidth="1"/>
+    <col min="21" max="23" width="11.5" style="1"/>
+    <col min="24" max="24" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6066,32 +6107,33 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="22" t="s">
         <v>480</v>
       </c>
-      <c r="K1" s="23"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
       <c r="N1" s="23"/>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="36" t="s">
         <v>481</v>
       </c>
-      <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
-      <c r="R1" s="5"/>
+      <c r="R1" s="24"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="42" t="s">
+      <c r="T1" s="5"/>
+      <c r="U1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="42"/>
       <c r="V1" s="42"/>
       <c r="W1" s="42"/>
       <c r="X1" s="42"/>
       <c r="Y1" s="42"/>
-    </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15">
+      <c r="Z1" s="42"/>
+    </row>
+    <row r="2" spans="1:26" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -6104,10 +6146,10 @@
       <c r="D2" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="45">
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" s="14" customFormat="1" ht="45">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -6123,65 +6165,68 @@
       <c r="E3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="43" t="s">
+        <v>669</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="V3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="W3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="X3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="Y3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="34" customFormat="1">
+    <row r="4" spans="1:26" s="34" customFormat="1">
       <c r="A4" s="34" t="b">
         <v>0</v>
       </c>
@@ -6191,10 +6236,11 @@
       <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="F4" s="44"/>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:25" s="34" customFormat="1">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:26" s="34" customFormat="1">
       <c r="B5" s="34" t="s">
         <v>22</v>
       </c>
@@ -6204,15 +6250,16 @@
       <c r="E5" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="F5" s="44"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:25" s="34" customFormat="1">
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" s="34" customFormat="1">
       <c r="A6" s="34" t="b">
         <v>1</v>
       </c>
@@ -6229,16 +6276,16 @@
       <c r="E6" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:25" s="34" customFormat="1">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" s="34" customFormat="1">
       <c r="B7" s="34" t="s">
         <v>22</v>
       </c>
@@ -6248,24 +6295,24 @@
       <c r="E7" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="G7" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="I7" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="J7" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" s="34" customFormat="1">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" s="34" customFormat="1">
       <c r="B8" s="34" t="s">
         <v>23</v>
       </c>
@@ -6276,33 +6323,36 @@
         <v>49</v>
       </c>
       <c r="F8" s="34" t="s">
+        <v>670</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="34">
+      <c r="I8" s="34">
         <v>30</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
+      <c r="J8" s="4"/>
       <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
         <v>70</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>20</v>
       </c>
-      <c r="M8" s="3">
-        <f>(K8-J8)/6</f>
+      <c r="N8" s="3">
+        <f>(L8-K8)/6</f>
         <v>11.666666666666666</v>
       </c>
-      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="34" t="s">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="34" customFormat="1">
+    <row r="9" spans="1:26" s="34" customFormat="1">
       <c r="B9" s="34" t="s">
         <v>22</v>
       </c>
@@ -6313,22 +6363,22 @@
       <c r="E9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="G9" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="34">
+      <c r="I9" s="34">
         <v>150</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:25" s="34" customFormat="1">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" s="34" customFormat="1">
       <c r="B10" s="34" t="s">
         <v>22</v>
       </c>
@@ -6338,22 +6388,22 @@
       <c r="E10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="G10" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="34">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="34">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:25" s="34" customFormat="1">
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" s="34" customFormat="1">
       <c r="B11" s="34" t="s">
         <v>22</v>
       </c>
@@ -6363,22 +6413,22 @@
       <c r="E11" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="G11" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="34">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="34">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:25" s="34" customFormat="1">
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" s="34" customFormat="1">
       <c r="B12" s="34" t="s">
         <v>22</v>
       </c>
@@ -6388,22 +6438,22 @@
       <c r="E12" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="G12" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:25" s="34" customFormat="1">
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" s="34" customFormat="1">
       <c r="B13" s="34" t="s">
         <v>22</v>
       </c>
@@ -6413,22 +6463,22 @@
       <c r="E13" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="G13" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="34">
+      <c r="I13" s="34">
         <v>15</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:25" s="34" customFormat="1">
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" s="34" customFormat="1">
       <c r="B14" s="34" t="s">
         <v>22</v>
       </c>
@@ -6438,22 +6488,22 @@
       <c r="E14" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="G14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="34">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:25" s="34" customFormat="1">
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" s="34" customFormat="1">
       <c r="B15" s="34" t="s">
         <v>22</v>
       </c>
@@ -6463,22 +6513,22 @@
       <c r="E15" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="G15" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="34">
+      <c r="I15" s="34">
         <v>1</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:25" s="34" customFormat="1">
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" s="34" customFormat="1">
       <c r="A16" s="34" t="b">
         <v>1</v>
       </c>
@@ -6495,9 +6545,9 @@
       <c r="E16" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:18" s="34" customFormat="1">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:19" s="34" customFormat="1">
       <c r="B17" s="34" t="s">
         <v>23</v>
       </c>
@@ -6508,33 +6558,36 @@
         <v>78</v>
       </c>
       <c r="F17" s="34" t="s">
+        <v>671</v>
+      </c>
+      <c r="G17" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="34">
+      <c r="I17" s="34">
         <v>90</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="34">
-        <v>0</v>
-      </c>
+      <c r="J17" s="4"/>
       <c r="K17" s="34">
+        <v>0</v>
+      </c>
+      <c r="L17" s="34">
         <v>359</v>
       </c>
-      <c r="L17" s="34">
+      <c r="M17" s="34">
         <v>180</v>
       </c>
-      <c r="M17" s="3">
-        <f>(K17-J17)/6</f>
+      <c r="N17" s="3">
+        <f>(L17-K17)/6</f>
         <v>59.833333333333336</v>
       </c>
-      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="34" t="s">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="34" customFormat="1" ht="15">
+    <row r="18" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A18" s="17" t="b">
         <v>1</v>
       </c>
@@ -6551,11 +6604,10 @@
       <c r="E18" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="33"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -6563,8 +6615,9 @@
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
-    </row>
-    <row r="19" spans="1:18" s="34" customFormat="1" ht="15">
+      <c r="R18" s="33"/>
+    </row>
+    <row r="19" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>23</v>
@@ -6576,35 +6629,38 @@
       <c r="E19" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="45" t="s">
+        <v>672</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17">
+      <c r="H19" s="17"/>
+      <c r="I19" s="17">
         <v>13</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="33">
-        <v>0</v>
-      </c>
+      <c r="J19" s="17"/>
       <c r="K19" s="33">
+        <v>0</v>
+      </c>
+      <c r="L19" s="33">
         <v>50</v>
       </c>
-      <c r="L19" s="17">
+      <c r="M19" s="17">
         <v>25</v>
       </c>
-      <c r="M19" s="3">
-        <f>(K19-J19)/6</f>
+      <c r="N19" s="3">
+        <f>(L19-K19)/6</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="33"/>
+      <c r="O19" s="3"/>
       <c r="P19" s="33"/>
-      <c r="Q19" s="33" t="s">
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="34" customFormat="1" ht="15">
+    <row r="20" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>22</v>
@@ -6616,15 +6672,14 @@
       <c r="E20" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="G20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17">
-        <v>0</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="33"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -6632,8 +6687,9 @@
       <c r="O20" s="33"/>
       <c r="P20" s="33"/>
       <c r="Q20" s="33"/>
-    </row>
-    <row r="21" spans="1:18" s="34" customFormat="1" ht="15">
+      <c r="R20" s="33"/>
+    </row>
+    <row r="21" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A21" s="17"/>
       <c r="B21" s="17" t="s">
         <v>22</v>
@@ -6645,15 +6701,14 @@
       <c r="E21" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="G21" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
-        <v>0</v>
-      </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="33"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -6661,8 +6716,9 @@
       <c r="O21" s="33"/>
       <c r="P21" s="33"/>
       <c r="Q21" s="33"/>
-    </row>
-    <row r="22" spans="1:18" s="34" customFormat="1" ht="15">
+      <c r="R21" s="33"/>
+    </row>
+    <row r="22" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>22</v>
@@ -6674,15 +6730,14 @@
       <c r="E22" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="G22" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
-        <v>0</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="33"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
@@ -6690,8 +6745,9 @@
       <c r="O22" s="33"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="33"/>
-    </row>
-    <row r="23" spans="1:18" s="34" customFormat="1" ht="15">
+      <c r="R22" s="33"/>
+    </row>
+    <row r="23" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A23" s="17" t="b">
         <v>1</v>
       </c>
@@ -6708,11 +6764,10 @@
       <c r="E23" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="33"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
       <c r="M23" s="33"/>
@@ -6720,8 +6775,9 @@
       <c r="O23" s="33"/>
       <c r="P23" s="33"/>
       <c r="Q23" s="33"/>
-    </row>
-    <row r="24" spans="1:18" s="34" customFormat="1" ht="15">
+      <c r="R23" s="33"/>
+    </row>
+    <row r="24" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>23</v>
@@ -6733,36 +6789,39 @@
       <c r="E24" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="45" t="s">
+        <v>673</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+      <c r="H24" s="17"/>
+      <c r="I24" s="17">
         <v>30</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="33">
+      <c r="J24" s="17"/>
+      <c r="K24" s="33">
         <v>10</v>
       </c>
-      <c r="K24" s="33">
+      <c r="L24" s="33">
         <v>80</v>
       </c>
-      <c r="L24" s="17">
+      <c r="M24" s="17">
         <v>50</v>
       </c>
-      <c r="M24" s="33"/>
       <c r="N24" s="33"/>
-      <c r="O24" s="33" t="s">
+      <c r="O24" s="33"/>
+      <c r="P24" s="33" t="s">
         <v>629</v>
       </c>
-      <c r="P24" s="33" t="s">
+      <c r="Q24" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="Q24" s="33" t="s">
+      <c r="R24" s="33" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="34" customFormat="1" ht="15">
+    <row r="25" spans="1:19" s="34" customFormat="1" ht="15">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>22</v>
@@ -6774,15 +6833,14 @@
       <c r="E25" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="G25" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17">
-        <v>0</v>
-      </c>
-      <c r="I25" s="17"/>
-      <c r="J25" s="33"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17"/>
       <c r="K25" s="33"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
@@ -6790,8 +6848,9 @@
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
-    </row>
-    <row r="26" spans="1:18" s="33" customFormat="1" ht="15">
+      <c r="R25" s="33"/>
+    </row>
+    <row r="26" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>22</v>
@@ -6803,16 +6862,17 @@
       <c r="E26" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="34"/>
+      <c r="G26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:18" s="33" customFormat="1" ht="15">
+      <c r="H26" s="17"/>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>22</v>
@@ -6824,16 +6884,17 @@
       <c r="E27" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="34"/>
+      <c r="G27" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17">
-        <v>0</v>
-      </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:18" s="33" customFormat="1" ht="15">
+      <c r="H27" s="17"/>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A28" s="17" t="b">
         <v>1</v>
       </c>
@@ -6850,13 +6911,14 @@
       <c r="E28" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
-      <c r="R28" s="34"/>
-    </row>
-    <row r="29" spans="1:18" s="33" customFormat="1" ht="15">
+      <c r="J28" s="17"/>
+      <c r="S28" s="34"/>
+    </row>
+    <row r="29" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>23</v>
@@ -6868,33 +6930,36 @@
       <c r="E29" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="45" t="s">
+        <v>674</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+      <c r="H29" s="17"/>
+      <c r="I29" s="17">
         <v>0.4</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="33">
+      <c r="J29" s="17"/>
+      <c r="K29" s="33">
         <v>0.05</v>
       </c>
-      <c r="K29" s="33">
+      <c r="L29" s="33">
         <v>0.95</v>
       </c>
-      <c r="L29" s="17">
+      <c r="M29" s="17">
         <v>0.4</v>
       </c>
-      <c r="M29" s="3">
-        <f>(K29-J29)/6</f>
+      <c r="N29" s="3">
+        <f>(L29-K29)/6</f>
         <v>0.15</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="Q29" s="33" t="s">
+      <c r="O29" s="3"/>
+      <c r="R29" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="33" customFormat="1" ht="15">
+    <row r="30" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>22</v>
@@ -6906,16 +6971,17 @@
       <c r="E30" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="34"/>
+      <c r="G30" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="H30" s="17"/>
+      <c r="I30" s="17">
         <v>30</v>
       </c>
-      <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:18" s="33" customFormat="1" ht="15">
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A31" s="17"/>
       <c r="B31" s="17" t="s">
         <v>22</v>
@@ -6927,18 +6993,19 @@
       <c r="E31" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="34"/>
+      <c r="G31" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="17"/>
+      <c r="I31" s="17" t="s">
         <v>630</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="J31" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="33" customFormat="1" ht="15">
+    <row r="32" spans="1:19" s="33" customFormat="1" ht="15">
       <c r="A32" s="17" t="b">
         <v>1</v>
       </c>
@@ -6955,13 +7022,14 @@
       <c r="E32" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
-      <c r="R32" s="34"/>
-    </row>
-    <row r="33" spans="1:19" s="33" customFormat="1" ht="15">
+      <c r="J32" s="17"/>
+      <c r="S32" s="34"/>
+    </row>
+    <row r="33" spans="1:20" s="33" customFormat="1" ht="15">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>22</v>
@@ -6973,19 +7041,20 @@
       <c r="E33" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="34"/>
+      <c r="G33" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="17"/>
+      <c r="I33" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="J33" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="Q33" s="34"/>
-    </row>
-    <row r="34" spans="1:19" s="33" customFormat="1" ht="15">
+      <c r="R33" s="34"/>
+    </row>
+    <row r="34" spans="1:20" s="33" customFormat="1" ht="15">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>22</v>
@@ -6997,505 +7066,531 @@
       <c r="E34" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="34"/>
+      <c r="G34" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="17"/>
+      <c r="I34" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="J34" s="17" t="s">
         <v>438</v>
       </c>
-      <c r="Q34" s="34"/>
-    </row>
-    <row r="35" spans="1:19" customFormat="1" ht="15">
+      <c r="R34" s="34"/>
+    </row>
+    <row r="35" spans="1:20" customFormat="1" ht="15">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:19" customFormat="1" ht="15">
+      <c r="L35" s="17"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:20" customFormat="1" ht="15">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="3"/>
+      <c r="L36" s="17"/>
+      <c r="O36" s="17"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="1"/>
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19" customFormat="1" ht="15">
+      <c r="Q36" s="3"/>
+      <c r="R36" s="1"/>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="1:20" customFormat="1" ht="15">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:19" customFormat="1" ht="15">
+      <c r="L37" s="17"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:20" customFormat="1" ht="15">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:19" customFormat="1" ht="15">
+      <c r="L38" s="17"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:20" customFormat="1" ht="15">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="F39" s="34"/>
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
-      <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="1:19" customFormat="1" ht="15">
+      <c r="L39" s="17"/>
+      <c r="R39" s="1"/>
+    </row>
+    <row r="40" spans="1:20" customFormat="1" ht="15">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
-      <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:19" customFormat="1" ht="15">
+      <c r="L40" s="17"/>
+      <c r="R40" s="1"/>
+    </row>
+    <row r="41" spans="1:20" customFormat="1" ht="15">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
+      <c r="F41" s="34"/>
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
-      <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="1:19" customFormat="1" ht="15">
+      <c r="L41" s="17"/>
+      <c r="R41" s="1"/>
+    </row>
+    <row r="42" spans="1:20" customFormat="1" ht="15">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
+      <c r="F42" s="34"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
-      <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" customFormat="1" ht="15">
+      <c r="L42" s="17"/>
+      <c r="R42" s="1"/>
+    </row>
+    <row r="43" spans="1:20" customFormat="1" ht="15">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
+      <c r="F43" s="34"/>
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
-      <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="1:19" customFormat="1" ht="15">
+      <c r="L43" s="17"/>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44" spans="1:20" customFormat="1" ht="15">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
-      <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="1:19" customFormat="1" ht="15">
+      <c r="L44" s="17"/>
+      <c r="R44" s="1"/>
+    </row>
+    <row r="45" spans="1:20" customFormat="1" ht="15">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="F45" s="34"/>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
-      <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="1:19" customFormat="1" ht="15">
+      <c r="L45" s="17"/>
+      <c r="R45" s="1"/>
+    </row>
+    <row r="46" spans="1:20" customFormat="1" ht="15">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
+      <c r="F46" s="34"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
-      <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="1:19" customFormat="1" ht="15">
+      <c r="L46" s="17"/>
+      <c r="R46" s="1"/>
+    </row>
+    <row r="47" spans="1:20" customFormat="1" ht="15">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="F47" s="34"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
-      <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="1:19" customFormat="1" ht="15">
+      <c r="L47" s="17"/>
+      <c r="R47" s="1"/>
+    </row>
+    <row r="48" spans="1:20" customFormat="1" ht="15">
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
+      <c r="F48" s="34"/>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
-      <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:25" customFormat="1" ht="15">
+      <c r="L48" s="17"/>
+      <c r="R48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" customFormat="1" ht="15">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
+      <c r="F49" s="34"/>
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
-      <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="1:25" customFormat="1" ht="15">
+      <c r="L49" s="17"/>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" customFormat="1" ht="15">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
+      <c r="F50" s="34"/>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
-      <c r="L50" s="3"/>
+      <c r="L50" s="17"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="1"/>
-      <c r="S50" s="1"/>
-    </row>
-    <row r="51" spans="1:25" customFormat="1" ht="15">
+      <c r="Q50" s="3"/>
+      <c r="R50" s="1"/>
+      <c r="T50" s="1"/>
+    </row>
+    <row r="51" spans="1:26" customFormat="1" ht="15">
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
+      <c r="F51" s="34"/>
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
-      <c r="L51" s="25"/>
+      <c r="L51" s="17"/>
       <c r="M51" s="25"/>
       <c r="N51" s="25"/>
       <c r="O51" s="25"/>
       <c r="P51" s="25"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="25"/>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="1"/>
       <c r="S51" s="25"/>
       <c r="T51" s="25"/>
       <c r="U51" s="25"/>
       <c r="V51" s="25"/>
-    </row>
-    <row r="52" spans="1:25" customFormat="1" ht="15">
+      <c r="W51" s="25"/>
+    </row>
+    <row r="52" spans="1:26" customFormat="1" ht="15">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
+      <c r="F52" s="34"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
-      <c r="M52" s="25"/>
+      <c r="M52" s="17"/>
       <c r="N52" s="25"/>
       <c r="O52" s="25"/>
       <c r="P52" s="25"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="1"/>
       <c r="S52" s="25"/>
       <c r="T52" s="25"/>
       <c r="U52" s="25"/>
       <c r="V52" s="25"/>
-    </row>
-    <row r="53" spans="1:25" customFormat="1" ht="15">
+      <c r="W52" s="25"/>
+    </row>
+    <row r="53" spans="1:26" customFormat="1" ht="15">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
+      <c r="F53" s="34"/>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
-      <c r="L53" s="26"/>
+      <c r="L53" s="17"/>
       <c r="M53" s="26"/>
       <c r="N53" s="26"/>
-      <c r="O53" s="3"/>
+      <c r="O53" s="26"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="25"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="1"/>
       <c r="S53" s="25"/>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
       <c r="V53" s="25"/>
-    </row>
-    <row r="54" spans="1:25" customFormat="1" ht="15">
+      <c r="W53" s="25"/>
+    </row>
+    <row r="54" spans="1:26" customFormat="1" ht="15">
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
+      <c r="F54" s="34"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
-      <c r="L54" s="25"/>
+      <c r="L54" s="17"/>
       <c r="M54" s="25"/>
       <c r="N54" s="25"/>
       <c r="O54" s="25"/>
       <c r="P54" s="25"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="1"/>
       <c r="S54" s="25"/>
       <c r="T54" s="25"/>
       <c r="U54" s="25"/>
       <c r="V54" s="25"/>
-    </row>
-    <row r="55" spans="1:25" customFormat="1" ht="15">
+      <c r="W54" s="25"/>
+    </row>
+    <row r="55" spans="1:26" customFormat="1" ht="15">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+      <c r="F55" s="34"/>
       <c r="G55" s="17"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
-      <c r="M55" s="25"/>
+      <c r="M55" s="17"/>
       <c r="N55" s="25"/>
       <c r="O55" s="25"/>
       <c r="P55" s="25"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="1"/>
       <c r="S55" s="25"/>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
       <c r="V55" s="25"/>
-    </row>
-    <row r="56" spans="1:25" customFormat="1" ht="15">
+      <c r="W55" s="25"/>
+    </row>
+    <row r="56" spans="1:26" customFormat="1" ht="15">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
+      <c r="F56" s="34"/>
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
       <c r="J56" s="17"/>
       <c r="K56" s="17"/>
-      <c r="L56" s="26"/>
+      <c r="L56" s="17"/>
       <c r="M56" s="26"/>
       <c r="N56" s="26"/>
-      <c r="O56" s="3"/>
+      <c r="O56" s="26"/>
       <c r="P56" s="3"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="25"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="1"/>
       <c r="S56" s="25"/>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
       <c r="V56" s="25"/>
-    </row>
-    <row r="57" spans="1:25" customFormat="1" ht="15">
+      <c r="W56" s="25"/>
+    </row>
+    <row r="57" spans="1:26" customFormat="1" ht="15">
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="F57" s="34"/>
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
-      <c r="L57" s="25"/>
+      <c r="L57" s="17"/>
       <c r="M57" s="25"/>
       <c r="N57" s="25"/>
       <c r="O57" s="25"/>
       <c r="P57" s="25"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="25"/>
+      <c r="Q57" s="25"/>
+      <c r="R57" s="1"/>
       <c r="S57" s="25"/>
       <c r="T57" s="25"/>
       <c r="U57" s="25"/>
       <c r="V57" s="25"/>
-    </row>
-    <row r="58" spans="1:25" customFormat="1" ht="15">
+      <c r="W57" s="25"/>
+    </row>
+    <row r="58" spans="1:26" customFormat="1" ht="15">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
+      <c r="F58" s="34"/>
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
       <c r="J58" s="17"/>
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
-      <c r="M58" s="25"/>
+      <c r="M58" s="17"/>
       <c r="N58" s="25"/>
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="25"/>
+      <c r="Q58" s="25"/>
+      <c r="R58" s="1"/>
       <c r="S58" s="25"/>
       <c r="T58" s="25"/>
       <c r="U58" s="25"/>
       <c r="V58" s="25"/>
-    </row>
-    <row r="59" spans="1:25" customFormat="1" ht="15">
+      <c r="W58" s="25"/>
+    </row>
+    <row r="59" spans="1:26" customFormat="1" ht="15">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
+      <c r="F59" s="34"/>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
-      <c r="L59" s="26"/>
+      <c r="L59" s="17"/>
       <c r="M59" s="26"/>
       <c r="N59" s="26"/>
-      <c r="O59" s="3"/>
+      <c r="O59" s="26"/>
       <c r="P59" s="3"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="25"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="1"/>
       <c r="S59" s="25"/>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
       <c r="V59" s="25"/>
-    </row>
-    <row r="60" spans="1:25" customFormat="1" ht="15">
+      <c r="W59" s="25"/>
+    </row>
+    <row r="60" spans="1:26" customFormat="1" ht="15">
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="F60" s="34"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
-      <c r="L60" s="25"/>
+      <c r="L60" s="17"/>
       <c r="M60" s="25"/>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="25"/>
+      <c r="Q60" s="25"/>
+      <c r="R60" s="1"/>
       <c r="S60" s="25"/>
       <c r="T60" s="25"/>
       <c r="U60" s="25"/>
       <c r="V60" s="25"/>
-    </row>
-    <row r="61" spans="1:25" ht="15">
+      <c r="W60" s="25"/>
+    </row>
+    <row r="61" spans="1:26" ht="15">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
       <c r="L61" s="17"/>
-      <c r="M61" s="25"/>
+      <c r="M61" s="17"/>
       <c r="N61" s="25"/>
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
-      <c r="R61" s="25"/>
+      <c r="Q61" s="25"/>
       <c r="S61" s="25"/>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -7503,25 +7598,25 @@
       <c r="W61" s="25"/>
       <c r="X61" s="25"/>
       <c r="Y61" s="25"/>
-    </row>
-    <row r="62" spans="1:25" ht="15">
+      <c r="Z61" s="25"/>
+    </row>
+    <row r="62" spans="1:26" ht="15">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
-      <c r="L62" s="26"/>
+      <c r="L62" s="17"/>
       <c r="M62" s="26"/>
       <c r="N62" s="26"/>
-      <c r="O62" s="3"/>
+      <c r="O62" s="26"/>
       <c r="P62" s="3"/>
-      <c r="R62" s="25"/>
+      <c r="Q62" s="3"/>
       <c r="S62" s="25"/>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -7529,14 +7624,14 @@
       <c r="W62" s="25"/>
       <c r="X62" s="25"/>
       <c r="Y62" s="25"/>
-    </row>
-    <row r="63" spans="1:25">
+      <c r="Z62" s="25"/>
+    </row>
+    <row r="63" spans="1:26">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63" s="33"/>
       <c r="D63" s="33"/>
       <c r="E63"/>
-      <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
@@ -7544,17 +7639,17 @@
       <c r="K63"/>
       <c r="L63"/>
       <c r="M63"/>
-      <c r="W63" s="25"/>
+      <c r="N63"/>
       <c r="X63" s="25"/>
       <c r="Y63" s="25"/>
-    </row>
-    <row r="64" spans="1:25">
+      <c r="Z63" s="25"/>
+    </row>
+    <row r="64" spans="1:26">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64" s="33"/>
       <c r="D64" s="33"/>
       <c r="E64"/>
-      <c r="F64"/>
       <c r="G64"/>
       <c r="H64"/>
       <c r="I64"/>
@@ -7562,17 +7657,17 @@
       <c r="K64"/>
       <c r="L64"/>
       <c r="M64"/>
-      <c r="W64" s="25"/>
+      <c r="N64"/>
       <c r="X64" s="25"/>
       <c r="Y64" s="25"/>
-    </row>
-    <row r="65" spans="1:25">
+      <c r="Z64" s="25"/>
+    </row>
+    <row r="65" spans="1:26">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65" s="33"/>
       <c r="D65" s="33"/>
       <c r="E65"/>
-      <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
       <c r="I65"/>
@@ -7580,103 +7675,104 @@
       <c r="K65"/>
       <c r="L65"/>
       <c r="M65"/>
-      <c r="W65" s="25"/>
+      <c r="N65"/>
       <c r="X65" s="25"/>
       <c r="Y65" s="25"/>
-    </row>
-    <row r="66" spans="1:25">
+      <c r="Z65" s="25"/>
+    </row>
+    <row r="66" spans="1:26">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66" s="33"/>
       <c r="D66"/>
       <c r="E66"/>
-      <c r="F66"/>
       <c r="G66"/>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66"/>
-      <c r="N66" s="3"/>
+      <c r="M66"/>
       <c r="O66" s="3"/>
-      <c r="Q66" s="25"/>
+      <c r="P66" s="3"/>
       <c r="R66" s="25"/>
-      <c r="V66" s="25"/>
+      <c r="S66" s="25"/>
       <c r="W66" s="25"/>
       <c r="X66" s="25"/>
-    </row>
-    <row r="67" spans="1:25">
+      <c r="Y66" s="25"/>
+    </row>
+    <row r="67" spans="1:26">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67" s="33"/>
       <c r="D67"/>
       <c r="E67"/>
-      <c r="F67"/>
       <c r="G67"/>
       <c r="H67"/>
       <c r="I67"/>
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67"/>
-      <c r="V67" s="25"/>
+      <c r="M67"/>
       <c r="W67" s="25"/>
       <c r="X67" s="25"/>
-    </row>
-    <row r="68" spans="1:25">
+      <c r="Y67" s="25"/>
+    </row>
+    <row r="68" spans="1:26">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68" s="33"/>
       <c r="D68"/>
       <c r="E68"/>
-      <c r="F68"/>
       <c r="G68"/>
       <c r="H68"/>
       <c r="I68"/>
       <c r="J68"/>
       <c r="K68"/>
       <c r="L68"/>
-      <c r="V68" s="25"/>
+      <c r="M68"/>
       <c r="W68" s="25"/>
       <c r="X68" s="25"/>
-    </row>
-    <row r="69" spans="1:25">
+      <c r="Y68" s="25"/>
+    </row>
+    <row r="69" spans="1:26">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69" s="33"/>
       <c r="D69"/>
       <c r="E69"/>
-      <c r="F69"/>
       <c r="G69"/>
       <c r="H69"/>
       <c r="I69"/>
       <c r="J69"/>
       <c r="K69"/>
       <c r="L69"/>
-      <c r="V69" s="25"/>
+      <c r="M69"/>
       <c r="W69" s="25"/>
       <c r="X69" s="25"/>
-    </row>
-    <row r="70" spans="1:25">
+      <c r="Y69" s="25"/>
+    </row>
+    <row r="70" spans="1:26">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70" s="33"/>
       <c r="D70"/>
       <c r="E70"/>
-      <c r="F70"/>
       <c r="G70"/>
       <c r="H70"/>
       <c r="I70"/>
       <c r="J70"/>
       <c r="K70"/>
       <c r="L70"/>
-      <c r="V70" s="25"/>
+      <c r="M70"/>
       <c r="W70" s="25"/>
       <c r="X70" s="25"/>
-    </row>
-    <row r="71" spans="1:25" customFormat="1">
+      <c r="Y70" s="25"/>
+    </row>
+    <row r="71" spans="1:26" customFormat="1">
       <c r="C71" s="33"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="1"/>
+      <c r="F71" s="34"/>
+      <c r="K71" s="4"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -7687,23 +7783,25 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
-    </row>
-    <row r="72" spans="1:25" customFormat="1" ht="15">
+      <c r="V71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" customFormat="1" ht="15">
       <c r="C72" s="33"/>
-      <c r="J72" s="4"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="3"/>
+      <c r="F72" s="34"/>
+      <c r="K72" s="4"/>
+      <c r="N72" s="17"/>
       <c r="O72" s="3"/>
-      <c r="P72" s="1"/>
-      <c r="R72" s="1"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
-    </row>
-    <row r="73" spans="1:25" customFormat="1">
+      <c r="V72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" customFormat="1">
       <c r="C73" s="33"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="1"/>
+      <c r="F73" s="34"/>
+      <c r="K73" s="4"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
@@ -7714,55 +7812,56 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
-    </row>
-    <row r="74" spans="1:25">
+      <c r="V73" s="1"/>
+    </row>
+    <row r="74" spans="1:26">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74" s="33"/>
       <c r="D74"/>
       <c r="E74"/>
-      <c r="F74"/>
       <c r="G74"/>
       <c r="H74"/>
       <c r="I74"/>
-      <c r="J74" s="4"/>
-    </row>
-    <row r="75" spans="1:25">
+      <c r="J74"/>
+      <c r="K74" s="4"/>
+    </row>
+    <row r="75" spans="1:26">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75" s="33"/>
       <c r="D75"/>
       <c r="E75"/>
-      <c r="F75"/>
       <c r="G75"/>
       <c r="H75"/>
       <c r="I75"/>
-      <c r="J75" s="4"/>
-    </row>
-    <row r="76" spans="1:25">
+      <c r="J75"/>
+      <c r="K75" s="4"/>
+    </row>
+    <row r="76" spans="1:26">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76" s="33"/>
       <c r="D76"/>
       <c r="E76"/>
-      <c r="F76"/>
       <c r="G76"/>
       <c r="H76"/>
       <c r="I76"/>
-      <c r="J76" s="4"/>
-    </row>
-    <row r="77" spans="1:25" customFormat="1">
+      <c r="J76"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="1:26" customFormat="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="34"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="34"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-      <c r="I77" s="4"/>
+      <c r="I77" s="1"/>
       <c r="J77" s="4"/>
-      <c r="K77" s="1"/>
+      <c r="K77" s="4"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
@@ -7770,77 +7869,88 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
-    </row>
-    <row r="78" spans="1:25" customFormat="1">
+      <c r="S77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" customFormat="1">
       <c r="A78" s="1"/>
       <c r="C78" s="33"/>
-      <c r="M78" s="1"/>
+      <c r="F78" s="34"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
-    </row>
-    <row r="79" spans="1:25" customFormat="1" ht="15">
+      <c r="S78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" customFormat="1" ht="15">
       <c r="A79" s="17"/>
       <c r="C79" s="33"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="3"/>
+      <c r="F79" s="34"/>
+      <c r="N79" s="1"/>
       <c r="O79" s="3"/>
-      <c r="P79" s="1"/>
+      <c r="P79" s="3"/>
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
-    </row>
-    <row r="80" spans="1:25" customFormat="1">
+      <c r="S79" s="1"/>
+    </row>
+    <row r="80" spans="1:26" customFormat="1">
       <c r="C80" s="33"/>
-    </row>
-    <row r="81" spans="1:24" customFormat="1">
+      <c r="F80" s="34"/>
+    </row>
+    <row r="81" spans="1:25" customFormat="1">
       <c r="C81" s="33"/>
-      <c r="N81" s="3"/>
+      <c r="F81" s="34"/>
       <c r="O81" s="3"/>
-      <c r="R81" s="1"/>
-    </row>
-    <row r="82" spans="1:24" customFormat="1">
+      <c r="P81" s="3"/>
+      <c r="S81" s="1"/>
+    </row>
+    <row r="82" spans="1:25" customFormat="1">
       <c r="C82" s="33"/>
-      <c r="N82" s="3"/>
+      <c r="F82" s="34"/>
       <c r="O82" s="3"/>
-      <c r="R82" s="1"/>
-    </row>
-    <row r="83" spans="1:24" customFormat="1">
+      <c r="P82" s="3"/>
+      <c r="S82" s="1"/>
+    </row>
+    <row r="83" spans="1:25" customFormat="1">
       <c r="C83" s="33"/>
-    </row>
-    <row r="84" spans="1:24" customFormat="1">
+      <c r="F83" s="34"/>
+    </row>
+    <row r="84" spans="1:25" customFormat="1">
       <c r="C84" s="33"/>
-      <c r="N84" s="3"/>
+      <c r="F84" s="34"/>
       <c r="O84" s="3"/>
-      <c r="R84" s="1"/>
-    </row>
-    <row r="85" spans="1:24" customFormat="1">
+      <c r="P84" s="3"/>
+      <c r="S84" s="1"/>
+    </row>
+    <row r="85" spans="1:25" customFormat="1">
       <c r="C85" s="33"/>
-    </row>
-    <row r="86" spans="1:24" customFormat="1">
+      <c r="F85" s="34"/>
+    </row>
+    <row r="86" spans="1:25" customFormat="1">
       <c r="C86" s="33"/>
-      <c r="N86" s="3"/>
+      <c r="F86" s="34"/>
       <c r="O86" s="3"/>
-      <c r="R86" s="1"/>
-    </row>
-    <row r="87" spans="1:24" customFormat="1">
+      <c r="P86" s="3"/>
+      <c r="S86" s="1"/>
+    </row>
+    <row r="87" spans="1:25" customFormat="1">
       <c r="C87" s="33"/>
-    </row>
-    <row r="88" spans="1:24" customFormat="1">
+      <c r="F87" s="34"/>
+    </row>
+    <row r="88" spans="1:25" customFormat="1">
       <c r="C88" s="33"/>
-      <c r="G88" s="1"/>
-      <c r="N88" s="3"/>
+      <c r="F88" s="34"/>
+      <c r="H88" s="1"/>
       <c r="O88" s="3"/>
-      <c r="R88" s="1"/>
-    </row>
-    <row r="89" spans="1:24">
+      <c r="P88" s="3"/>
+      <c r="S88" s="1"/>
+    </row>
+    <row r="89" spans="1:25">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89" s="33"/>
       <c r="D89"/>
       <c r="E89"/>
-      <c r="F89"/>
       <c r="G89"/>
       <c r="H89"/>
       <c r="I89"/>
@@ -7856,27 +7966,29 @@
       <c r="S89"/>
       <c r="T89"/>
       <c r="U89"/>
-      <c r="V89" s="25"/>
+      <c r="V89"/>
       <c r="W89" s="25"/>
       <c r="X89" s="25"/>
-    </row>
-    <row r="90" spans="1:24" customFormat="1">
+      <c r="Y89" s="25"/>
+    </row>
+    <row r="90" spans="1:25" customFormat="1">
       <c r="C90" s="33"/>
-      <c r="N90" s="3"/>
+      <c r="F90" s="34"/>
       <c r="O90" s="3"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="25"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="1"/>
       <c r="R90" s="25"/>
-    </row>
-    <row r="91" spans="1:24">
+      <c r="S90" s="25"/>
+    </row>
+    <row r="91" spans="1:25">
       <c r="C91" s="34"/>
-      <c r="H91" s="1"/>
-      <c r="J91" s="4"/>
+      <c r="I91" s="1"/>
+      <c r="K91" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Z15"/>
+  <autoFilter ref="A2:AA15"/>
   <mergeCells count="1">
-    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="U1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7890,90 +8002,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="1"/>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="34" customFormat="1" ht="18">
+    <row r="1" spans="1:13" s="34" customFormat="1" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="5"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15">
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
         <v>466</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>675</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>467</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="J2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:13" s="14" customFormat="1" ht="45">
+      <c r="A3" s="14" t="s">
         <v>648</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="B3" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>650</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>651</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>468</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>468</v>
@@ -7982,233 +8105,504 @@
         <v>468</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>654</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="K3" s="10" t="s">
+    </row>
+    <row r="4" spans="1:13" s="34" customFormat="1">
+      <c r="A4" s="33" t="s">
         <v>655</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="B4" s="33" t="s">
+        <v>677</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="34" customFormat="1">
-      <c r="A4" s="33" t="s">
+      <c r="D4" s="33" t="s">
         <v>657</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>658</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="F4" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="F4" s="33" t="b">
-        <v>1</v>
       </c>
       <c r="G4" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="33" t="b">
+        <v>0</v>
+      </c>
       <c r="J4" s="33"/>
       <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:12" s="34" customFormat="1">
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:13" s="34" customFormat="1">
       <c r="A5" s="33" t="s">
+        <v>658</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>678</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>659</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>660</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>661</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>662</v>
-      </c>
-      <c r="D5" s="33" t="s">
+      <c r="E5" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="33" t="b">
-        <v>0</v>
-      </c>
       <c r="G5" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="33" t="b">
+        <v>0</v>
+      </c>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
-    </row>
-    <row r="6" spans="1:12" s="34" customFormat="1">
+      <c r="M5" s="33"/>
+    </row>
+    <row r="6" spans="1:13" s="34" customFormat="1">
       <c r="A6" s="33" t="s">
+        <v>661</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>662</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>663</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>664</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>665</v>
-      </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="F6" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="F6" s="33" t="b">
-        <v>1</v>
       </c>
       <c r="G6" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="35"/>
       <c r="K6" s="33"/>
-    </row>
-    <row r="7" spans="1:12" s="34" customFormat="1">
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:13" s="34" customFormat="1">
       <c r="A7" s="33" t="s">
+        <v>664</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>665</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>666</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>667</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>668</v>
-      </c>
-      <c r="D7" s="33" t="s">
+      <c r="E7" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="F7" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="F7" s="33" t="b">
-        <v>1</v>
       </c>
       <c r="G7" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="35"/>
       <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="G8"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:12" customFormat="1">
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="33"/>
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="33"/>
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="33"/>
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="33"/>
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="33"/>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="33"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="33"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:13" customFormat="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" customFormat="1">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" customFormat="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" customFormat="1">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" customFormat="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" customFormat="1">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" customFormat="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" customFormat="1">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" customFormat="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" customFormat="1">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" customFormat="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="G23"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="G27"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="G30"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="33"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22" s="33"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="B23" s="33"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" s="33"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="33"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="33"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" s="33"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="33"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="33"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="33"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="33"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" s="33"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="33"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="33"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="33"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="33"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="33"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="33"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="33"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="33"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="33"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="33"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="33"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="33"/>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="33"/>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="33"/>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="33"/>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="33"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="33"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="33"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="33"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="33"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="33"/>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="33"/>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="33"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="33"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="33"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="33"/>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="33"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="33"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="33"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="33"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="33"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="33"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="33"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="33"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="33"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="33"/>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="33"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="33"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="33"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="33"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="33"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="33"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="33"/>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="33"/>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="33"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="33"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="33"/>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="33"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="33"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="33"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="33"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="33"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="33"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="33"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="33"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="33"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="33"/>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="33"/>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="33"/>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="33"/>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="33"/>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="33"/>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="33"/>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="33"/>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="33"/>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="33"/>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="33"/>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="33"/>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="33"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="33"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="33"/>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="33"/>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="33"/>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="33"/>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="33"/>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="33"/>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>